<commit_message>
Nuevo: Transport (acaRate, meta Data) Fuel Mode en Rx o Ex; Se elimina MultiSupply
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64015FD6-3FDD-4ED7-97A9-EC4DC6F10E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32485123-C18D-4607-890D-F16CCFA63C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
-    <sheet name="Supply" sheetId="2" r:id="rId2"/>
-    <sheet name="SupplyTrade" sheetId="3" r:id="rId3"/>
+    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Supply" sheetId="2" r:id="rId3"/>
     <sheet name="Sleeve" sheetId="7" r:id="rId4"/>
     <sheet name="Trade" sheetId="4" r:id="rId5"/>
     <sheet name="Transport" sheetId="5" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="95">
   <si>
     <t>Order</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Ref</t>
   </si>
   <si>
-    <t>MultiSupplyTrade</t>
-  </si>
-  <si>
     <t>MST1</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>Sell</t>
   </si>
   <si>
-    <t>Suppliers USA</t>
-  </si>
-  <si>
     <t>MARKET_Z</t>
   </si>
   <si>
@@ -221,18 +215,9 @@
     <t>TradeContractRef</t>
   </si>
   <si>
-    <t>OTRO_PTO</t>
-  </si>
-  <si>
     <t>OtroContrato</t>
   </si>
   <si>
-    <t>GenY</t>
-  </si>
-  <si>
-    <t>OTRO_MARKET</t>
-  </si>
-  <si>
     <t>Buy</t>
   </si>
   <si>
@@ -261,13 +246,94 @@
   </si>
   <si>
     <t>Sempra</t>
+  </si>
+  <si>
+    <t>Sleeve</t>
+  </si>
+  <si>
+    <t>SLEEVE_EAX_EXP</t>
+  </si>
+  <si>
+    <t>SLEEVE_EAX_IMP</t>
+  </si>
+  <si>
+    <t>JP. Morgan</t>
+  </si>
+  <si>
+    <t>J. Aron</t>
+  </si>
+  <si>
+    <t>Intraday</t>
+  </si>
+  <si>
+    <t>Mercuria</t>
+  </si>
+  <si>
+    <t>Exxon Mobil</t>
+  </si>
+  <si>
+    <t>JP Morgan</t>
+  </si>
+  <si>
+    <t>J.Aron</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>FuelMode</t>
+  </si>
+  <si>
+    <t>RxBase</t>
+  </si>
+  <si>
+    <t>ExBase</t>
+  </si>
+  <si>
+    <t>Planta</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>EBC</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>EAVIII</t>
+  </si>
+  <si>
+    <t>Bajío</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>HSC</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>AcaRate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +354,20 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +386,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -341,6 +437,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,82 +786,354 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="13">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="13">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="13">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="29" spans="1:4">
+      <c r="D29" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -759,189 +1142,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C52903-068A-4CF3-9AF2-E211C6D411FA}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="14.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="29">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>45982</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2">
-        <v>5300</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2.95</v>
-      </c>
-      <c r="K2" s="2">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="6:7">
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C52903-068A-4CF3-9AF2-E211C6D411FA}">
-  <dimension ref="A1:O8"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
     <col min="2" max="2" width="16.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
     <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" customWidth="1"/>
@@ -952,74 +1164,74 @@
     <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.453125" customWidth="1"/>
-    <col min="15" max="15" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="43.5">
+    <row r="1" spans="1:15" ht="29">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="J1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="29">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>45982</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1">
         <v>5300</v>
@@ -1031,42 +1243,42 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>45982</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1">
         <v>4700</v>
@@ -1078,42 +1290,42 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N3" s="1">
-        <v>0.6</v>
+        <v>1.6E-2</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>45982</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1">
         <v>4000</v>
@@ -1125,22 +1337,22 @@
         <v>0.02</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1">
-        <v>0.4</v>
+        <v>1.4E-2</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1158,6 +1370,578 @@
     <row r="8" spans="1:15">
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="15" max="15" width="11.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="29">
+      <c r="A1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2">
+        <v>18000</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2">
+        <v>15326</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2">
+        <v>17000</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M4" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2">
+        <v>21645</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2.37</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>43355</v>
+      </c>
+      <c r="L6">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>25000</v>
+      </c>
+      <c r="L7">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M7">
+        <v>0.04</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>5300</v>
+      </c>
+      <c r="L8">
+        <v>2.95</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>10000</v>
+      </c>
+      <c r="L9">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="F22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1169,84 +1953,86 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.5</v>
+      <c r="F3" s="10">
+        <v>0.02</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1259,7 +2045,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1273,42 +2059,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1342,130 +2128,305 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
-    <col min="8" max="8" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" customWidth="1"/>
+    <col min="10" max="10" width="20.26953125" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="H3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G2" s="2">
+      <c r="J3" s="2">
         <v>0.08</v>
       </c>
-      <c r="H2" s="2">
+      <c r="K3" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="H4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G3" s="2">
+      <c r="J4" s="2">
         <v>0.08</v>
       </c>
-      <c r="H3" s="2">
+      <c r="K4" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K5" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="H7" s="1"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="H8" s="1"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="H10" s="1"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,7 +2438,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1492,36 +2453,36 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D2" s="2">
-        <v>15300</v>
+        <v>15000</v>
       </c>
       <c r="E2" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Operaciones con parametros de PLANTA, Central y limpieza de código
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32485123-C18D-4607-890D-F16CCFA63C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EF51B-3DE5-4EAB-804A-EBE93752C5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="107">
   <si>
     <t>Order</t>
   </si>
@@ -308,9 +308,6 @@
     <t>EAVIII</t>
   </si>
   <si>
-    <t>Bajío</t>
-  </si>
-  <si>
     <t>Observación</t>
   </si>
   <si>
@@ -327,6 +324,45 @@
   </si>
   <si>
     <t>AcaRate</t>
+  </si>
+  <si>
+    <t>Esentia</t>
+  </si>
+  <si>
+    <t>Ramones</t>
+  </si>
+  <si>
+    <t>SISTRANGAS</t>
+  </si>
+  <si>
+    <t>Bajio - EAVIII</t>
+  </si>
+  <si>
+    <t>SBF</t>
+  </si>
+  <si>
+    <t>BAJIO</t>
+  </si>
+  <si>
+    <t>BAJJO</t>
+  </si>
+  <si>
+    <t>BAJIO.LT</t>
+  </si>
+  <si>
+    <t>NET MEX</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>AguaDulce</t>
+  </si>
+  <si>
+    <t>NET</t>
   </si>
 </sst>
 </file>
@@ -786,11 +822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -999,7 +1035,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1007,7 +1043,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -1015,7 +1051,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -1023,7 +1059,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1031,7 +1067,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1039,7 +1075,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1047,9 +1083,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>87</v>
@@ -1061,9 +1097,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>87</v>
@@ -1072,12 +1108,15 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>68</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>87</v>
@@ -1088,10 +1127,13 @@
       <c r="D25" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>87</v>
@@ -1100,12 +1142,15 @@
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>87</v>
@@ -1114,12 +1159,15 @@
         <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>87</v>
@@ -1128,12 +1176,92 @@
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="13">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="13">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="13">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="13">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="D29" s="1" t="s">
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="13">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1378,10 +1506,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1439,7 +1568,7 @@
         <v>29</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1847,101 +1976,275 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>90</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>91</v>
       </c>
       <c r="E15" s="4">
         <v>45982</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>25000</v>
+      </c>
+      <c r="L15">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M15">
+        <v>0.04</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="13"/>
       <c r="E16" s="4">
         <v>45982</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>5300</v>
+      </c>
+      <c r="L16">
+        <v>2.95</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="O16" s="13"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:14">
       <c r="A17" s="13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="C17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17">
+        <v>1000</v>
+      </c>
+      <c r="L17">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="13" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="C19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19">
+        <v>25000</v>
+      </c>
+      <c r="L19">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.04</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="13" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="C20" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20">
+        <v>5300</v>
+      </c>
+      <c r="L20">
+        <v>2.95</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>1000</v>
+      </c>
+      <c r="L21">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M21">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="F23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1950,90 +2253,271 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="8">
         <v>0.03</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="10">
+      <c r="H3" s="10">
         <v>0.02</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>34</v>
       </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2042,10 +2526,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2055,71 +2540,281 @@
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="5" max="5" width="24.90625" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2128,10 +2823,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2181,7 +2877,7 @@
         <v>44</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2341,7 +3037,7 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -2379,7 +3075,7 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -2413,20 +3109,134 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="K8" s="1"/>
-      <c r="L8" s="2"/>
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="K9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
+      <c r="A10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.4E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
+      <c r="A11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2435,85 +3245,180 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+    <col min="8" max="8" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>15000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="L10" s="1"/>
+      <c r="M10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nuevo modelo de Price(Formula) | Index + Adder para Sleeve y Supply; Location para Sleeve y Trade
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EF51B-3DE5-4EAB-804A-EBE93752C5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32F5C99-CA86-484A-A89E-4BC1C9C396F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,10 @@
     <sheet name="Transport" sheetId="5" r:id="rId6"/>
     <sheet name="Consume" sheetId="6" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="133">
   <si>
     <t>Order</t>
   </si>
@@ -182,9 +186,6 @@
     <t>Savi Energía</t>
   </si>
   <si>
-    <t>MeterLocation</t>
-  </si>
-  <si>
     <t>Planta_La_Estrella</t>
   </si>
   <si>
@@ -363,6 +364,87 @@
   </si>
   <si>
     <t>NET</t>
+  </si>
+  <si>
+    <t>TR_SE_CB</t>
+  </si>
+  <si>
+    <t>TR_CB_PLANT</t>
+  </si>
+  <si>
+    <t>TR_SES_SE</t>
+  </si>
+  <si>
+    <t>ESLP</t>
+  </si>
+  <si>
+    <t>SLEEVE_SES_EXP</t>
+  </si>
+  <si>
+    <t>SLEEVE_ESENTIA_IMP</t>
+  </si>
+  <si>
+    <t>MEXGAS</t>
+  </si>
+  <si>
+    <t>SBF_043_17</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ECHI</t>
+  </si>
+  <si>
+    <t>TC-001K</t>
+  </si>
+  <si>
+    <t>Adder</t>
+  </si>
+  <si>
+    <t>Buyback</t>
+  </si>
+  <si>
+    <t>Ogilby</t>
+  </si>
+  <si>
+    <t>Algodones</t>
+  </si>
+  <si>
+    <t>NBP</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>IEP</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Rmones</t>
+  </si>
+  <si>
+    <t>Index + 0,2</t>
+  </si>
+  <si>
+    <t>index + 1</t>
+  </si>
+  <si>
+    <t>index * .9</t>
   </si>
 </sst>
 </file>
@@ -403,7 +485,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +522,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -453,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -488,6 +588,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,11 +941,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -837,10 +956,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
@@ -854,7 +973,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -863,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -871,7 +990,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -888,7 +1007,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -897,15 +1016,15 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -914,15 +1033,15 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -939,7 +1058,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -956,7 +1075,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -973,298 +1092,455 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
+      <c r="A10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>85</v>
+      <c r="A11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="13">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" t="s">
-        <v>85</v>
+      <c r="A12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
+      <c r="A13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
+      <c r="A14" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C15" s="13">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C17" s="13">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C18" s="13">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="A19" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C19" s="13">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C20" s="13">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="A21" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="C21" s="13">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>86</v>
+      </c>
+      <c r="C22" s="13">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C23" s="13">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C24" s="13">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>69</v>
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="13">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="13">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1">
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>98</v>
+        <v>67</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="13">
+        <v>109</v>
+      </c>
+      <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="13" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="13">
+        <v>109</v>
+      </c>
+      <c r="C28">
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="13">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="C31" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="13">
-        <v>3</v>
+        <v>115</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="13">
-        <v>4</v>
+        <v>115</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="13">
+        <v>115</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35">
         <v>5</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1315,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>27</v>
@@ -1324,22 +1600,22 @@
         <v>28</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1374,10 +1650,10 @@
         <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>25</v>
@@ -1421,10 +1697,10 @@
         <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>25</v>
@@ -1450,7 +1726,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
@@ -1465,13 +1741,13 @@
         <v>0.02</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>25</v>
@@ -1506,11 +1782,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1520,16 +1796,18 @@
     <col min="5" max="5" width="16.7265625" customWidth="1"/>
     <col min="6" max="7" width="15.54296875" customWidth="1"/>
     <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" customWidth="1"/>
-    <col min="15" max="15" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" customWidth="1"/>
+    <col min="16" max="16" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29">
+    <row r="1" spans="1:16" ht="29">
       <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>11</v>
@@ -1558,22 +1836,25 @@
       <c r="K1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="11" t="s">
+      <c r="L1" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1597,7 +1878,7 @@
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>25</v>
@@ -1605,19 +1886,20 @@
       <c r="K2" s="2">
         <v>18000</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="19">
         <v>2.5750000000000002</v>
       </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -1641,7 +1923,7 @@
         <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>25</v>
@@ -1649,19 +1931,20 @@
       <c r="K3" s="2">
         <v>15326</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="19">
         <v>2.5750000000000002</v>
       </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -1685,7 +1968,7 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>25</v>
@@ -1693,19 +1976,22 @@
       <c r="K4" s="2">
         <v>17000</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="19">
         <v>2.5750000000000002</v>
       </c>
-      <c r="M4" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
@@ -1729,7 +2015,7 @@
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>25</v>
@@ -1737,19 +2023,20 @@
       <c r="K5" s="2">
         <v>21645</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="19">
         <v>2.37</v>
       </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="M5" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N5" s="21"/>
+      <c r="O5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -1773,7 +2060,7 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>25</v>
@@ -1781,19 +2068,20 @@
       <c r="K6">
         <v>43355</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="20">
         <v>0.77500000000000002</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1825,66 +2113,73 @@
       <c r="K7">
         <v>25000</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="20">
         <v>2.5750000000000002</v>
       </c>
-      <c r="M7">
-        <v>0.04</v>
-      </c>
-      <c r="N7" s="2" t="s">
+      <c r="M7" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="17">
         <v>45982</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K8">
-        <v>5300</v>
-      </c>
-      <c r="L8">
+      <c r="K8" s="18">
+        <v>-5000</v>
+      </c>
+      <c r="L8" s="20">
         <v>2.95</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2" t="s">
+      <c r="M8" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N8" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O8" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
         <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -1905,7 +2200,7 @@
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>25</v>
@@ -1913,91 +2208,92 @@
       <c r="K9">
         <v>10000</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="20">
         <v>2.5750000000000002</v>
       </c>
-      <c r="M9">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="M9" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N9" s="21"/>
+      <c r="O9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
         <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
         <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>85</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
         <v>84</v>
-      </c>
-      <c r="B12" t="s">
-        <v>85</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
         <v>84</v>
       </c>
-      <c r="B13" t="s">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="C15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="E15" s="4">
         <v>45982</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
@@ -2014,35 +2310,35 @@
       <c r="M15">
         <v>0.04</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="O15" s="13"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="O15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="E16" s="4">
         <v>45982</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" t="s">
         <v>23</v>
@@ -2059,38 +2355,38 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="O16" s="13"/>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="E17" s="4">
         <v>45982</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>25</v>
@@ -2104,34 +2400,37 @@
       <c r="M17">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="N17" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="4">
         <v>45982</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" t="s">
         <v>23</v>
@@ -2148,34 +2447,34 @@
       <c r="M19">
         <v>0.04</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" s="4">
         <v>45982</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" t="s">
         <v>23</v>
@@ -2192,37 +2491,37 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="4">
         <v>45982</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>25</v>
@@ -2236,15 +2535,59 @@
       <c r="M21">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>5300</v>
+      </c>
+      <c r="L24">
+        <v>2.95</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2253,271 +2596,275 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A29:A30"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
+    <col min="3" max="4" width="19.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="16.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="8">
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="8">
         <v>0.03</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="I3" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="10">
+      <c r="I5" s="10">
         <v>0.02</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="8" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="E7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+    <row r="8" spans="1:12">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2526,11 +2873,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2540,16 +2887,17 @@
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="5" max="5" width="24.90625" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="7" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>11</v>
@@ -2563,16 +2911,26 @@
       <c r="F1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2584,254 +2942,216 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H3" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H4" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H5" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
+    <row r="6" spans="1:12" ht="12" customHeight="1">
+      <c r="A6" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="23">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H6" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+    <row r="7" spans="1:12">
+      <c r="A7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="23">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
     <col min="4" max="4" width="15.81640625" customWidth="1"/>
     <col min="5" max="5" width="17.90625" customWidth="1"/>
     <col min="6" max="6" width="21.36328125" customWidth="1"/>
@@ -2842,12 +3162,12 @@
     <col min="12" max="12" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>11</v>
@@ -2865,7 +3185,7 @@
         <v>40</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>42</v>
@@ -2877,12 +3197,15 @@
         <v>44</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>92</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2903,7 +3226,7 @@
         <v>41</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="2">
         <v>7.0000000000000001E-3</v>
@@ -2917,10 +3240,13 @@
       <c r="L2" s="2">
         <v>1.4E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -2929,19 +3255,19 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="2">
         <v>7.0000000000000001E-3</v>
@@ -2955,13 +3281,16 @@
       <c r="L3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -2979,7 +3308,7 @@
         <v>41</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4" s="2">
         <v>7.0000000000000001E-3</v>
@@ -2993,31 +3322,34 @@
       <c r="L4" s="2">
         <v>1.4E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="2">
         <v>7.0000000000000001E-3</v>
@@ -3031,13 +3363,16 @@
       <c r="L5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -3055,7 +3390,7 @@
         <v>41</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="2">
         <v>7.0000000000000001E-3</v>
@@ -3070,30 +3405,30 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2">
         <v>7.0000000000000001E-3</v>
@@ -3108,118 +3443,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
+    <row r="8" spans="1:13">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="13" t="s">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I11" s="2">
         <v>7.0000000000000001E-3</v>
@@ -3231,12 +3540,140 @@
         <v>0.5</v>
       </c>
       <c r="L11" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
+    <row r="13" spans="1:13">
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3249,7 +3686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3264,10 +3701,10 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
@@ -3276,21 +3713,21 @@
         <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -3302,7 +3739,7 @@
         <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2">
         <v>15000</v>
@@ -3316,7 +3753,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -3324,48 +3761,48 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -3374,7 +3811,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="2">
         <v>1000</v>
@@ -3390,10 +3827,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -3402,7 +3839,7 @@
         <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="2">
         <v>5000</v>
@@ -3417,6 +3854,30 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.1</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="2"/>
     </row>

</xml_diff>

<commit_message>
Ahora incluye una Venta (Sell) con opción a transporte
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32F5C99-CA86-484A-A89E-4BC1C9C396F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C57A8-E363-422D-8DBA-8B4E9A807C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
-    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Sell" sheetId="8" r:id="rId2"/>
     <sheet name="Supply" sheetId="2" r:id="rId3"/>
-    <sheet name="Sleeve" sheetId="7" r:id="rId4"/>
-    <sheet name="Trade" sheetId="4" r:id="rId5"/>
-    <sheet name="Transport" sheetId="5" r:id="rId6"/>
-    <sheet name="Consume" sheetId="6" r:id="rId7"/>
+    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Sleeve" sheetId="7" r:id="rId5"/>
+    <sheet name="Trade" sheetId="4" r:id="rId6"/>
+    <sheet name="Transport" sheetId="5" r:id="rId7"/>
+    <sheet name="Consume" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Trade!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="134">
   <si>
     <t>Order</t>
   </si>
@@ -345,9 +346,6 @@
     <t>BAJIO</t>
   </si>
   <si>
-    <t>BAJJO</t>
-  </si>
-  <si>
     <t>BAJIO.LT</t>
   </si>
   <si>
@@ -417,12 +415,6 @@
     <t>GAP</t>
   </si>
   <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>IEP</t>
-  </si>
-  <si>
     <t>Pipeline</t>
   </si>
   <si>
@@ -445,6 +437,18 @@
   </si>
   <si>
     <t>index * .9</t>
+  </si>
+  <si>
+    <t>TR-BAJIO</t>
+  </si>
+  <si>
+    <t>CENAGAS</t>
+  </si>
+  <si>
+    <t>SELL_EAX</t>
+  </si>
+  <si>
+    <t>Ehrenberg</t>
   </si>
 </sst>
 </file>
@@ -553,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -606,7 +610,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,11 +944,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -971,7 +975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" hidden="1">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -988,7 +992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" hidden="1">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1005,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" hidden="1">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" hidden="1">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1039,7 +1043,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" hidden="1">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1073,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1090,7 +1094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1176,8 +1180,8 @@
       <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
+      <c r="E14" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1197,9 +1201,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" hidden="1">
       <c r="A16" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>86</v>
@@ -1211,9 +1215,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>86</v>
@@ -1225,12 +1229,12 @@
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>86</v>
@@ -1242,12 +1246,12 @@
         <v>7</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>86</v>
@@ -1262,9 +1266,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" hidden="1">
       <c r="A20" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>86</v>
@@ -1276,12 +1280,12 @@
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1">
       <c r="A21" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>86</v>
@@ -1293,12 +1297,12 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1">
       <c r="A22" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>86</v>
@@ -1313,12 +1317,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" hidden="1">
       <c r="A23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="13">
         <v>1</v>
@@ -1327,12 +1331,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" hidden="1">
       <c r="A24" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="13">
         <v>2</v>
@@ -1341,15 +1345,15 @@
         <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1">
       <c r="A25" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
@@ -1358,15 +1362,15 @@
         <v>67</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1">
       <c r="A26" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -1375,15 +1379,15 @@
         <v>67</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -1392,15 +1396,15 @@
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1">
       <c r="A28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -1409,15 +1413,15 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1">
       <c r="A29" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -1431,10 +1435,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" s="13">
         <v>1</v>
@@ -1445,10 +1449,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -1457,15 +1461,15 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -1474,15 +1478,15 @@
         <v>67</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="1">
         <v>4</v>
@@ -1491,15 +1495,15 @@
         <v>67</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1508,15 +1512,15 @@
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36">
         <v>6</v>
@@ -1525,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1540,12 +1544,919 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}"/>
+  <autoFilter ref="A1:E29" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="BAJIO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC381B67-0AA0-4433-85E0-5B9937ABBB10}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H2" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.08984375" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" customWidth="1"/>
+    <col min="16" max="16" width="11.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="29">
+      <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2">
+        <v>18000</v>
+      </c>
+      <c r="L2" s="19">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M2" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2">
+        <v>15326</v>
+      </c>
+      <c r="L3" s="19">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2">
+        <v>17000</v>
+      </c>
+      <c r="L4" s="19">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2">
+        <v>21645</v>
+      </c>
+      <c r="L5" s="19">
+        <v>2.37</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N5" s="21"/>
+      <c r="O5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>43355</v>
+      </c>
+      <c r="L6" s="20">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>25000</v>
+      </c>
+      <c r="L7" s="20">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="17">
+        <v>45982</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="18">
+        <v>-5000</v>
+      </c>
+      <c r="L8" s="20">
+        <v>2.95</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N8" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="20">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="N9" s="21"/>
+      <c r="O9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>25000</v>
+      </c>
+      <c r="L15">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M15">
+        <v>0.04</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>5300</v>
+      </c>
+      <c r="L16">
+        <v>2.95</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17">
+        <v>1000</v>
+      </c>
+      <c r="L17">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19">
+        <v>25000</v>
+      </c>
+      <c r="L19">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.04</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20">
+        <v>5300</v>
+      </c>
+      <c r="L20">
+        <v>2.95</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21">
+        <v>1000</v>
+      </c>
+      <c r="L21">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="M21">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45982</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>5300</v>
+      </c>
+      <c r="L24">
+        <v>2.95</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C52903-068A-4CF3-9AF2-E211C6D411FA}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -1780,827 +2691,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <dimension ref="A1:P24"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="3" max="3" width="20.90625" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.08984375" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" customWidth="1"/>
-    <col min="16" max="16" width="11.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="29">
-      <c r="A1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2">
-        <v>18000</v>
-      </c>
-      <c r="L2" s="19">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M2" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2">
-        <v>15326</v>
-      </c>
-      <c r="L3" s="19">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M3" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="2">
-        <v>17000</v>
-      </c>
-      <c r="L4" s="19">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M4" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="2">
-        <v>21645</v>
-      </c>
-      <c r="L5" s="19">
-        <v>2.37</v>
-      </c>
-      <c r="M5" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6">
-        <v>43355</v>
-      </c>
-      <c r="L6" s="20">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="M6" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7">
-        <v>25000</v>
-      </c>
-      <c r="L7" s="20">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M7" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="17">
-        <v>45982</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="18">
-        <v>-5000</v>
-      </c>
-      <c r="L8" s="20">
-        <v>2.95</v>
-      </c>
-      <c r="M8" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N8" s="21">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9">
-        <v>10000</v>
-      </c>
-      <c r="L9" s="20">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M9" s="21">
-        <v>0.03</v>
-      </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15">
-        <v>25000</v>
-      </c>
-      <c r="L15">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M15">
-        <v>0.04</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16">
-        <v>5300</v>
-      </c>
-      <c r="L16">
-        <v>2.95</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P16" s="13"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17">
-        <v>1000</v>
-      </c>
-      <c r="L17">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M17">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19">
-        <v>25000</v>
-      </c>
-      <c r="L19">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M19">
-        <v>0.04</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20">
-        <v>5300</v>
-      </c>
-      <c r="L20">
-        <v>2.95</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21">
-        <v>1000</v>
-      </c>
-      <c r="L21">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="M21">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="4">
-        <v>45982</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" t="s">
-        <v>112</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24">
-        <v>5300</v>
-      </c>
-      <c r="L24">
-        <v>2.95</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2625,7 +2722,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>59</v>
@@ -2640,13 +2737,13 @@
         <v>24</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>29</v>
@@ -2663,7 +2760,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>58</v>
@@ -2698,7 +2795,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>62</v>
@@ -2733,7 +2830,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>58</v>
@@ -2794,13 +2891,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>94</v>
@@ -2829,13 +2926,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>94</v>
@@ -2871,13 +2968,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:I1"/>
+      <selection pane="bottomLeft" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2912,16 +3009,16 @@
         <v>24</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>29</v>
@@ -2970,7 +3067,7 @@
         <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>33</v>
@@ -2998,13 +3095,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>33</v>
@@ -3022,7 +3119,7 @@
         <v>0.02</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>94</v>
@@ -3033,13 +3130,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -3048,7 +3145,7 @@
         <v>64</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="23">
         <v>2.5000000000000001E-2</v>
@@ -3066,19 +3163,19 @@
     </row>
     <row r="6" spans="1:12" ht="12" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>86</v>
@@ -3099,13 +3196,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>33</v>
@@ -3114,7 +3211,7 @@
         <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="23">
         <v>2.5000000000000001E-3</v>
@@ -3124,7 +3221,7 @@
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>34</v>
@@ -3140,13 +3237,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3200,7 +3297,7 @@
         <v>92</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3241,7 +3338,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="M2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -3282,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -3323,7 +3420,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="M4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3364,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3404,6 +3501,9 @@
       <c r="L6" s="2">
         <v>1.4E-3</v>
       </c>
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
@@ -3441,6 +3541,9 @@
       </c>
       <c r="L7" s="2">
         <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3457,7 +3560,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
@@ -3491,6 +3594,9 @@
       </c>
       <c r="L9" s="2">
         <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3507,19 +3613,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>94</v>
@@ -3542,10 +3648,13 @@
       <c r="L11" s="2">
         <v>1.4E-3</v>
       </c>
+      <c r="M11" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
         <v>86</v>
@@ -3587,19 +3696,19 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>94</v>
@@ -3622,16 +3731,19 @@
       <c r="L14" s="2">
         <v>1.4E-3</v>
       </c>
+      <c r="M14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>95</v>
@@ -3640,7 +3752,7 @@
         <v>94</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>64</v>
@@ -3660,19 +3772,49 @@
       <c r="L15" s="2">
         <v>0</v>
       </c>
+      <c r="M15" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="13" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>41</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>124</v>
+        <v>36</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3680,7 +3822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -3713,7 +3855,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>47</v>
@@ -3827,7 +3969,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
@@ -3855,10 +3997,10 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -3867,7 +4009,7 @@
         <v>45</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2">
         <v>3000</v>

</xml_diff>

<commit_message>
Operación de Sell en CUR-LR-EAX:; OK
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF357B3F-A95E-4088-BDC1-239710710C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD9FACD-73DB-4482-9D12-5DFB79D6C67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
-    <sheet name="Sell" sheetId="8" r:id="rId2"/>
-    <sheet name="Supply" sheetId="2" r:id="rId3"/>
-    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="Sleeve" sheetId="7" r:id="rId5"/>
-    <sheet name="Trade" sheetId="4" r:id="rId6"/>
-    <sheet name="Transport" sheetId="5" r:id="rId7"/>
+    <sheet name="Supply" sheetId="2" r:id="rId2"/>
+    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Sleeve" sheetId="7" r:id="rId4"/>
+    <sheet name="Trade" sheetId="4" r:id="rId5"/>
+    <sheet name="Transport" sheetId="5" r:id="rId6"/>
+    <sheet name="Sell" sheetId="8" r:id="rId7"/>
     <sheet name="Consume" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sleeve!$A$1:$M$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Supply!$A$1:$Q$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Trade!$B$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Transport!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Transport!$A$1:$N$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="151">
   <si>
     <t>Order</t>
   </si>
@@ -443,61 +443,67 @@
     <t>CENAGAS</t>
   </si>
   <si>
-    <t>SELL_EAX</t>
+    <t>Modo</t>
+  </si>
+  <si>
+    <t>CUR</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>CUR-A</t>
+  </si>
+  <si>
+    <t>CUR-B</t>
+  </si>
+  <si>
+    <t>A006F1</t>
+  </si>
+  <si>
+    <t>M006F1</t>
+  </si>
+  <si>
+    <t>LTF</t>
+  </si>
+  <si>
+    <t>SLEEVE_EBC_EXP</t>
+  </si>
+  <si>
+    <t>SLEEVE_EBC_IMP</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
+    <t>SP05</t>
+  </si>
+  <si>
+    <t>EntryLocation</t>
   </si>
   <si>
     <t>Ehrenberg</t>
   </si>
   <si>
-    <t>Modo</t>
-  </si>
-  <si>
-    <t>CUR</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>CUR-A</t>
-  </si>
-  <si>
-    <t>CUR-B</t>
-  </si>
-  <si>
-    <t>A006F1</t>
-  </si>
-  <si>
-    <t>M006F1</t>
-  </si>
-  <si>
-    <t>LTF</t>
-  </si>
-  <si>
-    <t>SLEEVE_EBC_EXP</t>
-  </si>
-  <si>
-    <t>SLEEVE_EBC_IMP</t>
-  </si>
-  <si>
-    <t>Eherenberg</t>
-  </si>
-  <si>
-    <t>Como se configura el transporte</t>
-  </si>
-  <si>
-    <t>No hay transporte</t>
-  </si>
-  <si>
-    <t>SELL</t>
-  </si>
-  <si>
-    <t>TC-01</t>
-  </si>
-  <si>
-    <t>TC-02</t>
-  </si>
-  <si>
-    <t>SP05</t>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>ClienteX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClienteX</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Sell - Cliente X</t>
+  </si>
+  <si>
+    <t>Tiene DiaGas y QtyMMBTU</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -660,6 +666,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -996,25 +1007,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49:E53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="5" max="5" width="26.1796875" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>81</v>
@@ -1032,9 +1044,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -1052,9 +1064,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -1072,9 +1084,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -1092,9 +1104,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -1112,29 +1124,32 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="27">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -1146,15 +1161,15 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -1166,35 +1181,35 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -1203,18 +1218,18 @@
         <v>84</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>139</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
@@ -1223,18 +1238,18 @@
         <v>84</v>
       </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
@@ -1243,18 +1258,18 @@
         <v>84</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
@@ -1263,18 +1278,18 @@
         <v>84</v>
       </c>
       <c r="D13" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
         <v>83</v>
@@ -1283,18 +1298,18 @@
         <v>84</v>
       </c>
       <c r="D14" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
         <v>83</v>
@@ -1303,35 +1318,38 @@
         <v>84</v>
       </c>
       <c r="D15" s="1">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="1">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="13">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" hidden="1">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>97</v>
@@ -1340,18 +1358,15 @@
         <v>85</v>
       </c>
       <c r="D17" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>97</v>
@@ -1360,18 +1375,18 @@
         <v>85</v>
       </c>
       <c r="D18" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>97</v>
@@ -1380,18 +1395,18 @@
         <v>85</v>
       </c>
       <c r="D19" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>97</v>
@@ -1400,18 +1415,18 @@
         <v>85</v>
       </c>
       <c r="D20" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>97</v>
@@ -1420,18 +1435,18 @@
         <v>85</v>
       </c>
       <c r="D21" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>97</v>
@@ -1440,15 +1455,18 @@
         <v>85</v>
       </c>
       <c r="D22" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>97</v>
@@ -1457,18 +1475,15 @@
         <v>85</v>
       </c>
       <c r="D23" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>97</v>
@@ -1477,18 +1492,18 @@
         <v>85</v>
       </c>
       <c r="D24" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>97</v>
@@ -1497,18 +1512,18 @@
         <v>85</v>
       </c>
       <c r="D25" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>97</v>
@@ -1517,18 +1532,18 @@
         <v>85</v>
       </c>
       <c r="D26" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>97</v>
@@ -1537,18 +1552,18 @@
         <v>85</v>
       </c>
       <c r="D27" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>97</v>
@@ -1557,35 +1572,38 @@
         <v>85</v>
       </c>
       <c r="D28" s="13">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1">
+      <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="13">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="13">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>107</v>
@@ -1594,18 +1612,15 @@
         <v>107</v>
       </c>
       <c r="D30" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>107</v>
@@ -1613,19 +1628,19 @@
       <c r="C31" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="1">
-        <v>3</v>
+      <c r="D31" s="13">
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>107</v>
@@ -1634,18 +1649,18 @@
         <v>107</v>
       </c>
       <c r="D32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="F32" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>107</v>
@@ -1653,19 +1668,19 @@
       <c r="C33" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D33">
-        <v>5</v>
+      <c r="D33" s="1">
+        <v>4</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>107</v>
@@ -1674,18 +1689,18 @@
         <v>107</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>107</v>
@@ -1694,18 +1709,18 @@
         <v>107</v>
       </c>
       <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="F35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>107</v>
@@ -1713,16 +1728,19 @@
       <c r="C36" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="13">
-        <v>1</v>
+      <c r="D36">
+        <v>7</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>9</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>107</v>
@@ -1731,18 +1749,15 @@
         <v>107</v>
       </c>
       <c r="D37" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>107</v>
@@ -1750,19 +1765,19 @@
       <c r="C38" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D38">
-        <v>5</v>
+      <c r="D38" s="13">
+        <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>107</v>
@@ -1771,18 +1786,18 @@
         <v>107</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>107</v>
@@ -1791,35 +1806,38 @@
         <v>107</v>
       </c>
       <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="13">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" hidden="1">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>113</v>
@@ -1827,19 +1845,16 @@
       <c r="C42" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D42">
-        <v>6</v>
+      <c r="D42" s="13">
+        <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>113</v>
@@ -1847,19 +1862,19 @@
       <c r="C43" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="1">
-        <v>3</v>
+      <c r="D43">
+        <v>6</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>113</v>
@@ -1868,18 +1883,18 @@
         <v>113</v>
       </c>
       <c r="D44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>113</v>
@@ -1887,19 +1902,19 @@
       <c r="C45" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D45">
-        <v>5</v>
+      <c r="D45" s="1">
+        <v>4</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>113</v>
@@ -1908,18 +1923,18 @@
         <v>113</v>
       </c>
       <c r="D46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>4</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>113</v>
@@ -1928,289 +1943,105 @@
         <v>113</v>
       </c>
       <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="18">
-        <v>1</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D50" s="18">
-        <v>2</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D51" s="24">
-        <v>3</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="24">
-        <v>4</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="18">
-        <v>5</v>
-      </c>
-      <c r="E53" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="18">
-        <v>6</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>147</v>
-      </c>
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F47" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}"/>
+  <autoFilter ref="A1:F48" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC381B67-0AA0-4433-85E0-5B9937ABBB10}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H2" s="23">
-        <v>0.02</v>
-      </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="M2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="23">
-        <v>2.34</v>
-      </c>
-      <c r="H3" s="23">
-        <v>0.02</v>
-      </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="M3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2228,7 +2059,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="29">
       <c r="A1" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
@@ -2279,9 +2110,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" hidden="1">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -2327,9 +2158,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" hidden="1">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2375,9 +2206,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" hidden="1">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -2425,9 +2256,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" hidden="1">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -2473,9 +2304,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" hidden="1">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -2521,9 +2352,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" hidden="1">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -2571,7 +2402,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -2624,7 +2455,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
@@ -2672,7 +2503,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -2720,7 +2551,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
@@ -2768,7 +2599,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
@@ -2818,7 +2649,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
@@ -2864,9 +2695,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" hidden="1">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>97</v>
@@ -2912,9 +2743,9 @@
       </c>
       <c r="Q14" s="13"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" hidden="1">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>97</v>
@@ -2960,9 +2791,9 @@
       </c>
       <c r="Q15" s="13"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" hidden="1">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>97</v>
@@ -3010,14 +2841,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" hidden="1">
       <c r="A17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" hidden="1">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>98</v>
@@ -3062,9 +2893,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" hidden="1">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>98</v>
@@ -3109,9 +2940,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" hidden="1">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>98</v>
@@ -3156,21 +2987,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" hidden="1">
       <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:16" hidden="1">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" hidden="1">
+      <c r="A23" t="s">
         <v>133</v>
-      </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" t="s">
-        <v>133</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" t="s">
-        <v>135</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>107</v>
@@ -3217,7 +3048,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="18" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>83</v>
@@ -3226,16 +3057,27 @@
         <v>84</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q23" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}"/>
+  <autoFilter ref="A1:Q24" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LR"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="EBC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C52903-068A-4CF3-9AF2-E211C6D411FA}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -3470,16 +3312,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3495,7 +3337,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
@@ -3536,7 +3378,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -3545,7 +3387,7 @@
         <v>84</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>116</v>
@@ -3574,7 +3416,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -3583,7 +3425,7 @@
         <v>84</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>117</v>
@@ -3612,34 +3454,34 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>85</v>
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>124</v>
+      <c r="E4" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="J4" s="8">
-        <v>0.03</v>
+        <v>2.5</v>
       </c>
       <c r="K4" s="8">
         <v>0.03</v>
@@ -3650,37 +3492,37 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>85</v>
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>93</v>
+      <c r="E5" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>92</v>
+        <v>63</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>64</v>
       </c>
       <c r="J5" s="10">
-        <v>0.02</v>
+        <v>2.5</v>
       </c>
       <c r="K5" s="10">
-        <v>0.02</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>34</v>
@@ -3688,37 +3530,37 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0.02</v>
+      <c r="I6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.03</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>34</v>
@@ -3726,16 +3568,16 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>93</v>
@@ -3763,25 +3605,100 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M7" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J8"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3798,7 +3715,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
@@ -3837,7 +3754,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -3874,7 +3791,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -3911,7 +3828,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>97</v>
@@ -3948,7 +3865,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>98</v>
@@ -3986,7 +3903,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>98</v>
@@ -4022,7 +3939,7 @@
     </row>
     <row r="7" spans="1:13" ht="12" customHeight="1">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>98</v>
@@ -4058,7 +3975,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>107</v>
@@ -4102,16 +4019,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2:N13"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4129,7 +4046,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>81</v>
@@ -4171,9 +4088,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" hidden="1">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -4215,9 +4132,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" hidden="1">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -4261,7 +4178,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -4270,7 +4187,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>36</v>
@@ -4305,7 +4222,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -4314,7 +4231,7 @@
         <v>84</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>66</v>
@@ -4347,9 +4264,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" hidden="1">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -4391,9 +4308,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" hidden="1">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -4435,9 +4352,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" hidden="1">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
         <v>97</v>
@@ -4479,9 +4396,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" hidden="1">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>98</v>
@@ -4523,9 +4440,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" hidden="1">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>98</v>
@@ -4564,9 +4481,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" hidden="1">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>107</v>
@@ -4608,9 +4525,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" hidden="1">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>107</v>
@@ -4652,9 +4569,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" hidden="1">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>83</v>
@@ -4697,7 +4614,110 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}"/>
+  <autoFilter ref="A1:N13" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LR"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="EBC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089709AD-E983-493A-A97B-8B77F3CEAF40}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="11" customFormat="1">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="25">
+        <v>46001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2">
+        <v>50000</v>
+      </c>
+      <c r="H2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I2">
+        <v>0.7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4707,26 +4727,26 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G9"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" customWidth="1"/>
-    <col min="9" max="9" width="25.26953125" customWidth="1"/>
+    <col min="5" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
+    <col min="10" max="10" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>81</v>
@@ -4741,21 +4761,24 @@
         <v>35</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -4770,21 +4793,24 @@
         <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>15000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -4799,21 +4825,24 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>15000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -4828,21 +4857,24 @@
         <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>15000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>5</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
         <v>83</v>
@@ -4850,12 +4882,15 @@
       <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="F5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -4863,12 +4898,15 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="F6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>97</v>
@@ -4883,23 +4921,26 @@
         <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>1000</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>0.1</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7" s="1"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
@@ -4913,24 +4954,25 @@
       <c r="E8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>5000</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0.1</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8" s="1"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
         <v>107</v>
@@ -4944,23 +4986,24 @@
       <c r="E9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>3000</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>0.1</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
+  <autoFilter ref="A1:O1" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios  en el excel para l Venta
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD9FACD-73DB-4482-9D12-5DFB79D6C67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DA4F6D-40A0-4E6E-95F8-A7387EC26EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="11550" yWindow="-16185" windowWidth="15975" windowHeight="10560" firstSheet="1" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="Consume" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$O$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="153">
   <si>
     <t>Order</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Cliente Y</t>
+  </si>
+  <si>
+    <t>Sell - Cliente Y</t>
   </si>
 </sst>
 </file>
@@ -612,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -670,7 +676,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1010,11 +1017,11 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1125,46 +1132,49 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="28">
         <v>5</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="27" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
+      <c r="D7" s="28">
+        <v>5</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1178,13 +1188,13 @@
         <v>41</v>
       </c>
       <c r="D8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1198,36 +1208,36 @@
         <v>41</v>
       </c>
       <c r="D9" s="1">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -1238,16 +1248,16 @@
         <v>84</v>
       </c>
       <c r="D11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -1258,16 +1268,16 @@
         <v>84</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1278,16 +1288,16 @@
         <v>84</v>
       </c>
       <c r="D13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -1298,16 +1308,16 @@
         <v>84</v>
       </c>
       <c r="D14" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -1318,16 +1328,16 @@
         <v>84</v>
       </c>
       <c r="D15" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -1338,30 +1348,33 @@
         <v>84</v>
       </c>
       <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1">
       <c r="A17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="13">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1">
@@ -1375,13 +1388,10 @@
         <v>85</v>
       </c>
       <c r="D18" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1">
@@ -1395,13 +1405,13 @@
         <v>85</v>
       </c>
       <c r="D19" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>69</v>
+      <c r="F19" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:6" hidden="1">
@@ -1415,13 +1425,13 @@
         <v>85</v>
       </c>
       <c r="D20" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>96</v>
+        <v>67</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1">
@@ -1435,13 +1445,13 @@
         <v>85</v>
       </c>
       <c r="D21" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1">
@@ -1455,18 +1465,18 @@
         <v>85</v>
       </c>
       <c r="D22" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>97</v>
@@ -1475,10 +1485,13 @@
         <v>85</v>
       </c>
       <c r="D23" s="13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1">
@@ -1492,13 +1505,10 @@
         <v>85</v>
       </c>
       <c r="D24" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1">
@@ -1512,13 +1522,13 @@
         <v>85</v>
       </c>
       <c r="D25" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1">
@@ -1532,13 +1542,13 @@
         <v>85</v>
       </c>
       <c r="D26" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" hidden="1">
@@ -1552,13 +1562,13 @@
         <v>85</v>
       </c>
       <c r="D27" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>104</v>
+        <v>4</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1">
@@ -1572,13 +1582,13 @@
         <v>85</v>
       </c>
       <c r="D28" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1">
@@ -1592,30 +1602,33 @@
         <v>85</v>
       </c>
       <c r="D29" s="13">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>10</v>
+      <c r="F29" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D30" s="13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" hidden="1">
@@ -1629,13 +1642,10 @@
         <v>107</v>
       </c>
       <c r="D31" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1">
@@ -1648,14 +1658,14 @@
       <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="1">
-        <v>3</v>
+      <c r="D32" s="13">
+        <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>108</v>
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1">
@@ -1669,13 +1679,13 @@
         <v>107</v>
       </c>
       <c r="D33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="9" t="s">
-        <v>109</v>
+      <c r="F33" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1">
@@ -1688,14 +1698,14 @@
       <c r="C34" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D34">
-        <v>5</v>
+      <c r="D34" s="1">
+        <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1">
@@ -1709,13 +1719,13 @@
         <v>107</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>112</v>
+        <v>4</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1">
@@ -1729,18 +1739,18 @@
         <v>107</v>
       </c>
       <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>10</v>
+      <c r="F36" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>107</v>
@@ -1748,11 +1758,14 @@
       <c r="C37" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="13">
-        <v>1</v>
+      <c r="D37">
+        <v>7</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1">
@@ -1766,13 +1779,10 @@
         <v>107</v>
       </c>
       <c r="D38" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1">
@@ -1785,14 +1795,14 @@
       <c r="C39" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D39">
-        <v>5</v>
+      <c r="D39" s="13">
+        <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:6" hidden="1">
@@ -1806,13 +1816,13 @@
         <v>107</v>
       </c>
       <c r="D40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
-        <v>112</v>
+        <v>4</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1">
@@ -1826,30 +1836,33 @@
         <v>107</v>
       </c>
       <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>10</v>
+      <c r="F41" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="13">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1">
@@ -1862,14 +1875,11 @@
       <c r="C43" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D43">
-        <v>6</v>
+      <c r="D43" s="13">
+        <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1">
@@ -1882,14 +1892,14 @@
       <c r="C44" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="1">
-        <v>3</v>
+      <c r="D44">
+        <v>6</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1">
@@ -1903,13 +1913,13 @@
         <v>113</v>
       </c>
       <c r="D45" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>109</v>
+      <c r="F45" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:6" hidden="1">
@@ -1922,14 +1932,14 @@
       <c r="C46" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D46">
-        <v>5</v>
+      <c r="D46" s="1">
+        <v>4</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>111</v>
+        <v>67</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1">
@@ -1943,13 +1953,13 @@
         <v>113</v>
       </c>
       <c r="D47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>112</v>
+        <v>4</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1">
@@ -1963,22 +1973,34 @@
         <v>113</v>
       </c>
       <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="18"/>
@@ -1986,15 +2008,15 @@
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
-      <c r="D52" s="24"/>
+      <c r="D52" s="18"/>
       <c r="E52" s="24"/>
-      <c r="F52" s="7"/>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="18"/>
@@ -2002,15 +2024,15 @@
       <c r="C53" s="18"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="9"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="D54" s="24"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="1"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="18"/>
@@ -2018,10 +2040,23 @@
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="24"/>
-      <c r="F55" s="18"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F48" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+  <autoFilter ref="A1:F49" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CUR"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="LR"/>
@@ -2039,9 +2074,9 @@
   </sheetPr>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8:L13"/>
+    <sheetView topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2051,6 +2086,7 @@
     <col min="6" max="6" width="16.7265625" customWidth="1"/>
     <col min="7" max="8" width="15.54296875" customWidth="1"/>
     <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" customWidth="1"/>
     <col min="13" max="13" width="13.08984375" customWidth="1"/>
     <col min="14" max="14" width="13.6328125" customWidth="1"/>
     <col min="16" max="16" width="14.54296875" customWidth="1"/>
@@ -2110,7 +2146,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -2206,7 +2242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -2256,7 +2292,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -2304,7 +2340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -2352,7 +2388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -2400,7 +2436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" hidden="1">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -2453,7 +2489,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" hidden="1">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -2501,7 +2537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" hidden="1">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -2549,7 +2585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" hidden="1">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -2597,7 +2633,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" hidden="1">
       <c r="A12" t="s">
         <v>137</v>
       </c>
@@ -2647,7 +2683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" hidden="1">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -3046,7 +3082,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" hidden="1">
       <c r="A24" s="18" t="s">
         <v>140</v>
       </c>
@@ -3069,7 +3105,7 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="EBC"/>
+        <filter val="EAX"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3314,14 +3350,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="8"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3376,7 +3412,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" hidden="1">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -3414,7 +3450,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" hidden="1">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -3528,7 +3564,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" hidden="1">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -3566,7 +3602,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" hidden="1">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -3604,7 +3640,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" hidden="1">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -3642,7 +3678,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" hidden="1">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -3685,6 +3721,18 @@
       <c r="C10" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M9" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CUR"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4026,9 +4074,9 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4088,7 +4136,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -4132,7 +4180,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -4176,7 +4224,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" hidden="1">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -4220,7 +4268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" hidden="1">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4569,7 +4617,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -4622,7 +4670,7 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="EBC"/>
+        <filter val="EAX"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4635,10 +4683,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4705,7 +4753,7 @@
         <v>146</v>
       </c>
       <c r="G2">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="H2">
         <v>2.2999999999999998</v>
@@ -4714,6 +4762,38 @@
         <v>0.7</v>
       </c>
       <c r="K2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="25">
+        <v>46001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>2.1</v>
+      </c>
+      <c r="I3">
+        <v>0.2</v>
+      </c>
+      <c r="K3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4724,14 +4804,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4799,7 +4879,7 @@
         <v>46</v>
       </c>
       <c r="H2" s="2">
-        <v>15000</v>
+        <v>68862</v>
       </c>
       <c r="I2" s="2">
         <v>5</v>
@@ -4831,7 +4911,7 @@
         <v>46</v>
       </c>
       <c r="H3" s="2">
-        <v>15000</v>
+        <v>68862</v>
       </c>
       <c r="I3" s="2">
         <v>5</v>
@@ -4840,7 +4920,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" hidden="1">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -4872,7 +4952,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" hidden="1">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -4888,7 +4968,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" hidden="1">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -4904,7 +4984,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" hidden="1">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -4938,7 +5018,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" hidden="1">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -4970,7 +5050,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" hidden="1">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -5003,7 +5083,23 @@
       <c r="O9" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
+  <autoFilter ref="A1:O9" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CUR"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="LR"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="EAX"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Primera versión con JoinFlow (dos flow se unen)
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DA4F6D-40A0-4E6E-95F8-A7387EC26EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B6C124-763E-4418-AD94-484DF1BBD39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="-16185" windowWidth="15975" windowHeight="10560" firstSheet="1" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$O$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="153">
   <si>
     <t>Order</t>
   </si>
@@ -500,9 +500,6 @@
     <t>Sell - Cliente X</t>
   </si>
   <si>
-    <t>Tiene DiaGas y QtyMMBTU</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>Sell - Cliente Y</t>
+  </si>
+  <si>
+    <t>JoinKey</t>
   </si>
 </sst>
 </file>
@@ -1017,11 +1017,11 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:E7"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1050,6 +1050,9 @@
       <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -1151,30 +1154,27 @@
         <v>148</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="28">
-        <v>5</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>149</v>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1188,13 +1188,13 @@
         <v>41</v>
       </c>
       <c r="D8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1208,33 +1208,33 @@
         <v>41</v>
       </c>
       <c r="D9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="D10" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1">
@@ -1248,13 +1248,13 @@
         <v>84</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:7" hidden="1">
@@ -1268,13 +1268,13 @@
         <v>84</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>135</v>
+        <v>67</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" hidden="1">
@@ -1288,13 +1288,13 @@
         <v>84</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>138</v>
+      <c r="F13" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1">
@@ -1308,13 +1308,13 @@
         <v>84</v>
       </c>
       <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>139</v>
+      <c r="F14" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1">
@@ -1328,13 +1328,13 @@
         <v>84</v>
       </c>
       <c r="D15" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" hidden="1">
@@ -1348,33 +1348,30 @@
         <v>84</v>
       </c>
       <c r="D16" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1">
       <c r="A17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="1">
-        <v>7</v>
+        <v>131</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1">
@@ -1388,10 +1385,13 @@
         <v>85</v>
       </c>
       <c r="D18" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1">
@@ -1405,13 +1405,13 @@
         <v>85</v>
       </c>
       <c r="D19" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>68</v>
+      <c r="F19" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" hidden="1">
@@ -1425,13 +1425,13 @@
         <v>85</v>
       </c>
       <c r="D20" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>69</v>
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1">
@@ -1445,13 +1445,13 @@
         <v>85</v>
       </c>
       <c r="D21" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1">
@@ -1465,18 +1465,18 @@
         <v>85</v>
       </c>
       <c r="D22" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>97</v>
@@ -1485,13 +1485,10 @@
         <v>85</v>
       </c>
       <c r="D23" s="13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1">
@@ -1505,10 +1502,13 @@
         <v>85</v>
       </c>
       <c r="D24" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1">
@@ -1522,13 +1522,13 @@
         <v>85</v>
       </c>
       <c r="D25" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1">
@@ -1542,13 +1542,13 @@
         <v>85</v>
       </c>
       <c r="D26" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" hidden="1">
@@ -1562,13 +1562,13 @@
         <v>85</v>
       </c>
       <c r="D27" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>96</v>
+        <v>7</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1">
@@ -1582,13 +1582,13 @@
         <v>85</v>
       </c>
       <c r="D28" s="13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1">
@@ -1602,33 +1602,30 @@
         <v>85</v>
       </c>
       <c r="D29" s="13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>105</v>
+        <v>9</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D30" s="13">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:6" hidden="1">
@@ -1642,10 +1639,13 @@
         <v>107</v>
       </c>
       <c r="D31" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1">
@@ -1658,14 +1658,14 @@
       <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13">
-        <v>2</v>
+      <c r="D32" s="1">
+        <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>103</v>
+        <v>67</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1">
@@ -1679,13 +1679,13 @@
         <v>107</v>
       </c>
       <c r="D33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>108</v>
+      <c r="F33" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1">
@@ -1698,14 +1698,14 @@
       <c r="C34" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>109</v>
+      <c r="F34" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1">
@@ -1719,13 +1719,13 @@
         <v>107</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>111</v>
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1">
@@ -1739,18 +1739,18 @@
         <v>107</v>
       </c>
       <c r="D36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>112</v>
+        <v>9</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>107</v>
@@ -1758,14 +1758,11 @@
       <c r="C37" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D37">
-        <v>7</v>
+      <c r="D37" s="13">
+        <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1">
@@ -1779,10 +1776,13 @@
         <v>107</v>
       </c>
       <c r="D38" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1">
@@ -1795,14 +1795,14 @@
       <c r="C39" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="13">
-        <v>2</v>
+      <c r="D39">
+        <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:6" hidden="1">
@@ -1816,13 +1816,13 @@
         <v>107</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>111</v>
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1">
@@ -1836,33 +1836,30 @@
         <v>107</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>112</v>
+        <v>9</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42">
-        <v>7</v>
+        <v>113</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1">
@@ -1875,11 +1872,14 @@
       <c r="C43" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="13">
-        <v>1</v>
+      <c r="D43">
+        <v>6</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>77</v>
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1">
@@ -1892,14 +1892,14 @@
       <c r="C44" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D44">
-        <v>6</v>
+      <c r="D44" s="1">
+        <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1">
@@ -1913,13 +1913,13 @@
         <v>113</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>108</v>
+      <c r="F45" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:6" hidden="1">
@@ -1932,14 +1932,14 @@
       <c r="C46" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>109</v>
+      <c r="F46" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1">
@@ -1953,13 +1953,13 @@
         <v>113</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>111</v>
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1">
@@ -1973,34 +1973,22 @@
         <v>113</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1">
-      <c r="A49" t="s">
-        <v>131</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49">
-        <v>7</v>
-      </c>
-      <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="18"/>
@@ -2008,15 +1996,15 @@
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="18"/>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="D52" s="24"/>
       <c r="E52" s="24"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="18"/>
@@ -2024,15 +2012,15 @@
       <c r="C53" s="18"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="7"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
-      <c r="D54" s="24"/>
+      <c r="D54" s="18"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="9"/>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="18"/>
@@ -2040,18 +2028,10 @@
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="24"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="18"/>
+      <c r="F55" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F49" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+  <autoFilter ref="A1:F48" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
     <filterColumn colId="0">
       <filters>
         <filter val="CUR"/>
@@ -4721,7 +4701,7 @@
         <v>65</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>114</v>
@@ -4767,7 +4747,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="25">
         <v>46001</v>
@@ -4782,7 +4762,7 @@
         <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3">
         <v>10000</v>
@@ -4809,7 +4789,7 @@
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>

</xml_diff>

<commit_message>
Ok el cambio de Planta x Path: FLowId = {Modo, Central, Path}
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B6C124-763E-4418-AD94-484DF1BBD39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381DFF3-8CF1-4649-A452-EAF32F18BF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,17 @@
     <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Sleeve" sheetId="7" r:id="rId4"/>
     <sheet name="Trade" sheetId="4" r:id="rId5"/>
-    <sheet name="Transport" sheetId="5" r:id="rId6"/>
-    <sheet name="Sell" sheetId="8" r:id="rId7"/>
-    <sheet name="Consume" sheetId="6" r:id="rId8"/>
+    <sheet name="Sell" sheetId="8" r:id="rId6"/>
+    <sheet name="Consume" sheetId="6" r:id="rId7"/>
+    <sheet name="Transport" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Consume!$A$1:$O$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Consume!$A$1:$O$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Transport!$A$1:$N$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Transport!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="162">
   <si>
     <t>Order</t>
   </si>
@@ -296,15 +296,9 @@
     <t>ExBase</t>
   </si>
   <si>
-    <t>Planta</t>
-  </si>
-  <si>
     <t>Central</t>
   </si>
   <si>
-    <t>LR</t>
-  </si>
-  <si>
     <t>EBC</t>
   </si>
   <si>
@@ -344,12 +338,6 @@
     <t>SBF</t>
   </si>
   <si>
-    <t>BAJIO</t>
-  </si>
-  <si>
-    <t>BAJIO.LT</t>
-  </si>
-  <si>
     <t>NET MEX</t>
   </si>
   <si>
@@ -455,9 +443,6 @@
     <t>CUR-A</t>
   </si>
   <si>
-    <t>CUR-B</t>
-  </si>
-  <si>
     <t>A006F1</t>
   </si>
   <si>
@@ -510,13 +495,55 @@
   </si>
   <si>
     <t>JoinKey</t>
+  </si>
+  <si>
+    <t>E104</t>
+  </si>
+  <si>
+    <t>SISTR</t>
+  </si>
+  <si>
+    <t>PEMEX</t>
+  </si>
+  <si>
+    <t>Pemex</t>
+  </si>
+  <si>
+    <t>MexGas</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>JOIN_ESLP</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Path1</t>
+  </si>
+  <si>
+    <t>Path2</t>
+  </si>
+  <si>
+    <t>Path3</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>E014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,6 +575,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1017,11 +1050,11 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1033,13 +1066,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -1051,18 +1084,18 @@
         <v>2</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1074,15 +1107,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" hidden="1">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -1094,15 +1127,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -1114,15 +1147,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -1134,15 +1167,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" s="27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="27" t="s">
         <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
       </c>
       <c r="D6" s="28">
         <v>5</v>
@@ -1151,21 +1184,21 @@
         <v>33</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -1177,15 +1210,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D8" s="1">
         <v>7</v>
@@ -1197,15 +1230,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" hidden="1">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D9" s="1">
         <v>8</v>
@@ -1219,13 +1252,13 @@
     </row>
     <row r="10" spans="1:7" hidden="1">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1239,13 +1272,13 @@
     </row>
     <row r="11" spans="1:7" hidden="1">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -1254,18 +1287,18 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" hidden="1">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
@@ -1274,18 +1307,18 @@
         <v>67</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:7" hidden="1">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -1294,18 +1327,18 @@
         <v>67</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D14" s="1">
         <v>5</v>
@@ -1314,18 +1347,18 @@
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -1339,13 +1372,13 @@
     </row>
     <row r="16" spans="1:7" hidden="1">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D16" s="1">
         <v>7</v>
@@ -1357,15 +1390,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
       </c>
       <c r="D17" s="13">
         <v>1</v>
@@ -1374,15 +1407,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1">
+    <row r="18" spans="1:7" hidden="1">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
@@ -1394,15 +1427,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>156</v>
       </c>
       <c r="D19" s="13">
         <v>3</v>
@@ -1414,15 +1447,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>156</v>
       </c>
       <c r="D20" s="13">
         <v>4</v>
@@ -1431,18 +1464,18 @@
         <v>4</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>156</v>
       </c>
       <c r="D21" s="13">
         <v>5</v>
@@ -1451,18 +1484,18 @@
         <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>156</v>
       </c>
       <c r="D22" s="13">
         <v>6</v>
@@ -1474,15 +1507,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>156</v>
       </c>
       <c r="D23" s="13">
         <v>1</v>
@@ -1491,15 +1524,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
       </c>
       <c r="D24" s="13">
         <v>2</v>
@@ -1508,18 +1541,18 @@
         <v>4</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>156</v>
       </c>
       <c r="D25" s="13">
         <v>3</v>
@@ -1528,18 +1561,18 @@
         <v>7</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
       </c>
       <c r="D26" s="13">
         <v>4</v>
@@ -1548,18 +1581,18 @@
         <v>4</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>156</v>
       </c>
       <c r="D27" s="13">
         <v>5</v>
@@ -1568,18 +1601,18 @@
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>156</v>
       </c>
       <c r="D28" s="13">
         <v>6</v>
@@ -1588,18 +1621,18 @@
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>156</v>
       </c>
       <c r="D29" s="13">
         <v>7</v>
@@ -1611,15 +1644,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C30" t="s">
+        <v>157</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
@@ -1627,136 +1660,148 @@
       <c r="E30" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1">
+      <c r="F30" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="13">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1">
-      <c r="A32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1">
+      <c r="G32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="1">
-        <v>4</v>
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1">
+        <v>77</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C34" t="s">
+        <v>158</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1">
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>159</v>
       </c>
       <c r="D36">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1">
+        <v>103</v>
+      </c>
+      <c r="G36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
+        <v>156</v>
       </c>
       <c r="D37" s="13">
         <v>1</v>
@@ -1765,222 +1810,165 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B38" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1">
+      <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="13">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" hidden="1">
-      <c r="A39" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" hidden="1">
-      <c r="A40" t="s">
-        <v>134</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40">
+    </row>
+    <row r="42" spans="1:7" hidden="1">
+      <c r="A42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42">
         <v>6</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" hidden="1">
-      <c r="A41" t="s">
-        <v>134</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D41">
+      <c r="F42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43">
         <v>7</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1">
-      <c r="A42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="13">
-        <v>1</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" hidden="1">
-      <c r="A43" t="s">
-        <v>131</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43">
-        <v>6</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" hidden="1">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="1">
-        <v>3</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" hidden="1">
-      <c r="A45" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="1">
-        <v>4</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" hidden="1">
-      <c r="A46" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D46">
-        <v>5</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" hidden="1">
-      <c r="A47" t="s">
-        <v>131</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47">
-        <v>6</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" hidden="1">
-      <c r="A48" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48">
-        <v>7</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="45" spans="1:7">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="18"/>
@@ -1990,48 +1978,8 @@
       <c r="E50" s="24"/>
       <c r="F50" s="18"/>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="18"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F48" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+  <autoFilter ref="A1:F43" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
     <filterColumn colId="0">
       <filters>
         <filter val="CUR"/>
@@ -2039,10 +1987,11 @@
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="LR"/>
+        <filter val="ESLP"/>
       </filters>
     </filterColumn>
   </autoFilter>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2052,11 +2001,11 @@
   <sheetPr filterMode="1">
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2075,13 +2024,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="29">
       <c r="A1" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -2111,30 +2060,30 @@
         <v>26</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>29</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" hidden="1">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -2174,15 +2123,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" hidden="1">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -2222,15 +2171,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" hidden="1">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -2266,21 +2215,21 @@
         <v>0.03</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" hidden="1">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2320,15 +2269,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" hidden="1">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -2368,15 +2317,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" hidden="1">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -2418,13 +2367,13 @@
     </row>
     <row r="8" spans="1:17" hidden="1">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -2466,18 +2415,18 @@
         <v>30</v>
       </c>
       <c r="Q8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:17" hidden="1">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -2519,13 +2468,13 @@
     </row>
     <row r="10" spans="1:17" hidden="1">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2567,13 +2516,13 @@
     </row>
     <row r="11" spans="1:17" hidden="1">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -2615,13 +2564,13 @@
     </row>
     <row r="12" spans="1:17" hidden="1">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -2657,7 +2606,7 @@
         <v>0.03</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>30</v>
@@ -2665,13 +2614,13 @@
     </row>
     <row r="13" spans="1:17" hidden="1">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -2713,31 +2662,31 @@
     </row>
     <row r="14" spans="1:17" hidden="1">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E14" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" s="4">
         <v>45982</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
         <v>23</v>
@@ -2755,37 +2704,37 @@
         <v>0.04</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17" hidden="1">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E15" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" s="4">
         <v>45982</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
         <v>72</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
         <v>23</v>
@@ -2803,37 +2752,37 @@
         <v>0</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:17" hidden="1">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E16" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4">
         <v>45982</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J16" t="s">
         <v>76</v>
@@ -2851,44 +2800,47 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:16" hidden="1">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:16" hidden="1">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E18" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F18" s="4">
         <v>45982</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H18" t="s">
         <v>19</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
@@ -2906,36 +2858,36 @@
         <v>0.04</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:16" hidden="1">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E19" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F19" s="4">
         <v>45982</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H19" t="s">
         <v>72</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
@@ -2953,36 +2905,36 @@
         <v>0</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:16" hidden="1">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>87</v>
-      </c>
       <c r="E20" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F20" s="4">
         <v>45982</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J20" t="s">
         <v>76</v>
@@ -3000,51 +2952,57 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:16" hidden="1">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>156</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:16" hidden="1">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>156</v>
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:16" hidden="1">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4">
         <v>45982</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
         <v>72</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>25</v>
@@ -3059,33 +3017,75 @@
         <v>0</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:16" hidden="1">
       <c r="A24" s="18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="4">
+        <v>45982</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" t="s">
+        <v>150</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25">
+        <v>2000</v>
+      </c>
+      <c r="M25">
+        <v>1.9</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q24" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
+  <autoFilter ref="A1:Q25" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
     <filterColumn colId="1">
       <filters>
-        <filter val="LR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="EAX"/>
+        <filter val="ESLP"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3335,9 +3335,9 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3353,19 +3353,19 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>59</v>
@@ -3380,13 +3380,13 @@
         <v>24</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>29</v>
@@ -3394,19 +3394,16 @@
     </row>
     <row r="2" spans="1:13" hidden="1">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>58</v>
@@ -3432,19 +3429,16 @@
     </row>
     <row r="3" spans="1:13" hidden="1">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>62</v>
@@ -3470,19 +3464,19 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>58</v>
@@ -3508,19 +3502,19 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>69</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>62</v>
@@ -3544,33 +3538,33 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J6" s="8">
         <v>0.03</v>
@@ -3582,30 +3576,30 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>64</v>
@@ -3622,25 +3616,23 @@
     </row>
     <row r="8" spans="1:13" hidden="1">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C8" s="13"/>
       <c r="D8" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
         <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -3660,28 +3652,26 @@
     </row>
     <row r="9" spans="1:13" hidden="1">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>107</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>64</v>
@@ -3705,11 +3695,6 @@
     <filterColumn colId="0">
       <filters>
         <filter val="CUR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="LR"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3724,15 +3709,14 @@
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L1"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="2" max="3" width="14.26953125" customWidth="1"/>
     <col min="4" max="4" width="14.453125" customWidth="1"/>
     <col min="6" max="6" width="24.90625" customWidth="1"/>
     <col min="7" max="7" width="15.08984375" customWidth="1"/>
@@ -3743,13 +3727,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -3764,16 +3748,16 @@
         <v>24</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>29</v>
@@ -3782,13 +3766,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3819,13 +3803,13 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3837,7 +3821,7 @@
         <v>64</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="23">
         <v>2.5000000000000001E-2</v>
@@ -3847,7 +3831,7 @@
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>34</v>
@@ -3856,16 +3840,16 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -3874,7 +3858,7 @@
         <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" s="23">
         <v>2.5000000000000001E-2</v>
@@ -3884,7 +3868,7 @@
       </c>
       <c r="J4" s="23"/>
       <c r="K4" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>34</v>
@@ -3893,16 +3877,16 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>33</v>
@@ -3920,10 +3904,10 @@
         <v>0.02</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>34</v>
@@ -3931,16 +3915,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>33</v>
@@ -3949,7 +3933,7 @@
         <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H6" s="23">
         <v>2.5000000000000001E-2</v>
@@ -3959,7 +3943,7 @@
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>34</v>
@@ -3967,25 +3951,25 @@
     </row>
     <row r="7" spans="1:13" ht="12" customHeight="1">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="23">
         <v>2.5000000000000001E-2</v>
@@ -3995,7 +3979,7 @@
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>34</v>
@@ -4003,16 +3987,16 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>33</v>
@@ -4021,7 +4005,7 @@
         <v>64</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H8" s="23">
         <v>2.5000000000000001E-3</v>
@@ -4031,15 +4015,47 @@
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="I9" s="23">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:L1" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}"/>
@@ -4048,617 +4064,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <sheetPr filterMode="1">
-    <tabColor theme="7"/>
-  </sheetPr>
-  <dimension ref="A1:N13"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2:K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" customWidth="1"/>
-    <col min="7" max="7" width="21.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1"/>
-    <col min="11" max="11" width="20.26953125" customWidth="1"/>
-    <col min="12" max="12" width="21.90625" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" hidden="1">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1">
-      <c r="A5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" hidden="1">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" hidden="1">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1">
-      <c r="A9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1">
-      <c r="A10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" hidden="1">
-      <c r="A11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" hidden="1">
-      <c r="A12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="N13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:N13" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="LR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="EAX"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089709AD-E983-493A-A97B-8B77F3CEAF40}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4686,10 +4091,10 @@
         <v>15</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>22</v>
@@ -4701,13 +4106,13 @@
         <v>65</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>29</v>
@@ -4715,22 +4120,22 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="26" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B2" s="25">
         <v>46001</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G2">
         <v>60000</v>
@@ -4742,27 +4147,27 @@
         <v>0.7</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="27" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B3" s="25">
         <v>46001</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G3">
         <v>10000</v>
@@ -4774,7 +4179,7 @@
         <v>0.2</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4782,16 +4187,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4806,13 +4211,13 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="14" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>11</v>
@@ -4821,10 +4226,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>47</v>
@@ -4838,13 +4243,13 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -4853,7 +4258,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -4870,13 +4275,13 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -4885,7 +4290,7 @@
         <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>46</v>
@@ -4900,15 +4305,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -4917,10 +4322,10 @@
         <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" s="2">
         <v>15000</v>
@@ -4932,47 +4337,53 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>156</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" hidden="1">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>156</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" hidden="1">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -4981,10 +4392,10 @@
         <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="2">
         <v>1000</v>
@@ -4998,88 +4409,725 @@
       <c r="N7" s="1"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" hidden="1">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8">
+        <v>832</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O8" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" customWidth="1"/>
+    <col min="12" max="12" width="21.90625" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
       <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5000</v>
-      </c>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" hidden="1">
-      <c r="A9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" s="2">
-        <v>3000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>5</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="K15" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O9" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CUR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="LR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="EAX"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N14" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Compila y ejecuta MultiFlo para ESLP con dos providers
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381DFF3-8CF1-4649-A452-EAF32F18BF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{E714AF85-4405-4118-B559-9BFF506FBD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
@@ -31,6 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Transport!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="161">
   <si>
     <t>Order</t>
   </si>
@@ -534,9 +535,6 @@
   </si>
   <si>
     <t>SP2</t>
-  </si>
-  <si>
-    <t>E014</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1051,8 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1781,12 +1779,12 @@
         <v>159</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" t="s">
         <v>103</v>
       </c>
       <c r="G36" t="s">
@@ -2004,8 +2002,8 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3045,7 +3043,7 @@
         <v>158</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>97</v>
@@ -4196,7 +4194,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4456,7 +4454,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5061,7 +5059,7 @@
         <v>98</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
OK ejecuta Join (merge) paths
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{E714AF85-4405-4118-B559-9BFF506FBD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{A2EB4B04-D507-4E2D-A07A-F4AF62F52452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Consume!$A$1:$O$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$F$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$G$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="161">
   <si>
     <t>Order</t>
   </si>
@@ -1050,16 +1050,16 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" sqref="A1:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="5" max="5" width="26.1796875" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1076,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" hidden="1">
@@ -1098,10 +1098,10 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1118,10 +1118,10 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1138,10 +1138,13 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1158,10 +1161,10 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1178,14 +1181,11 @@
       <c r="D6" s="28">
         <v>5</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="F6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="G6" s="27" t="s">
         <v>143</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" hidden="1">
@@ -1201,10 +1201,13 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1221,10 +1224,13 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1241,10 +1247,11 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1261,10 +1268,11 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1281,10 +1289,11 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1301,10 +1310,11 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1321,10 +1331,11 @@
       <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1341,10 +1352,11 @@
       <c r="D14" s="1">
         <v>5</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1361,10 +1373,11 @@
       <c r="D15" s="1">
         <v>6</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1381,10 +1394,11 @@
       <c r="D16" s="1">
         <v>7</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1401,7 +1415,8 @@
       <c r="D17" s="13">
         <v>1</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="13"/>
+      <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1418,10 +1433,11 @@
       <c r="D18" s="13">
         <v>2</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="13"/>
+      <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1438,10 +1454,11 @@
       <c r="D19" s="13">
         <v>3</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="13"/>
+      <c r="F19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1458,10 +1475,11 @@
       <c r="D20" s="13">
         <v>4</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="13"/>
+      <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1478,10 +1496,11 @@
       <c r="D21" s="13">
         <v>5</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="13"/>
+      <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1498,10 +1517,11 @@
       <c r="D22" s="13">
         <v>6</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="13"/>
+      <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1518,7 +1538,8 @@
       <c r="D23" s="13">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="13"/>
+      <c r="F23" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1535,10 +1556,11 @@
       <c r="D24" s="13">
         <v>2</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="13"/>
+      <c r="F24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1555,10 +1577,11 @@
       <c r="D25" s="13">
         <v>3</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="13"/>
+      <c r="F25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1575,10 +1598,11 @@
       <c r="D26" s="13">
         <v>4</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="13"/>
+      <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1595,10 +1619,11 @@
       <c r="D27" s="13">
         <v>5</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="13"/>
+      <c r="F27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1615,10 +1640,11 @@
       <c r="D28" s="13">
         <v>6</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1635,10 +1661,11 @@
       <c r="D29" s="13">
         <v>7</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1655,10 +1682,10 @@
       <c r="D30" s="13">
         <v>1</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1675,10 +1702,10 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1695,14 +1722,14 @@
       <c r="D32">
         <v>3</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>108</v>
-      </c>
-      <c r="G32" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1718,10 +1745,10 @@
       <c r="D33" s="13">
         <v>1</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="G33" s="13" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1738,10 +1765,10 @@
       <c r="D34">
         <v>2</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1758,14 +1785,14 @@
       <c r="D35">
         <v>3</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>153</v>
-      </c>
-      <c r="G35" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1781,14 +1808,14 @@
       <c r="D36">
         <v>3</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
+        <v>154</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>103</v>
-      </c>
-      <c r="G36" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:7" hidden="1">
@@ -1804,7 +1831,8 @@
       <c r="D37" s="13">
         <v>1</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="13"/>
+      <c r="F37" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1821,10 +1849,10 @@
       <c r="D38">
         <v>6</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1841,10 +1869,11 @@
       <c r="D39" s="1">
         <v>3</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1861,10 +1890,11 @@
       <c r="D40" s="1">
         <v>4</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="G40" s="9" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1881,10 +1911,10 @@
       <c r="D41">
         <v>5</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1901,10 +1931,10 @@
       <c r="D42">
         <v>6</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1921,10 +1951,10 @@
       <c r="D43">
         <v>7</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1933,16 +1963,18 @@
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="18"/>
@@ -1950,7 +1982,8 @@
       <c r="C47" s="18"/>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
-      <c r="F47" s="7"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="18"/>
@@ -1958,26 +1991,29 @@
       <c r="C48" s="18"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="F48" s="24"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="E49" s="18"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F43" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+  <autoFilter ref="A1:G43" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
     <filterColumn colId="0">
       <filters>
         <filter val="CUR"/>
@@ -2003,7 +2039,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23:L25"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4069,7 +4105,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4194,7 +4230,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4452,9 +4488,9 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Ya se tiene una forma de mostrar pos proceso; Single y Multi paht
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{A2EB4B04-D507-4E2D-A07A-F4AF62F52452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C73DCF9-604C-4561-A85F-0C45DC139401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Transport!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="161">
   <si>
     <t>Order</t>
   </si>
@@ -516,9 +515,6 @@
     <t>ABCD</t>
   </si>
   <si>
-    <t>JOIN_ESLP</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
@@ -535,6 +531,9 @@
   </si>
   <si>
     <t>SP2</t>
+  </si>
+  <si>
+    <t>JOIN_KEY</t>
   </si>
 </sst>
 </file>
@@ -649,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -700,9 +699,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1048,11 +1044,11 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1070,7 +1066,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -1085,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -1093,7 +1089,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1101,11 +1097,11 @@
       <c r="F2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -1113,7 +1109,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -1125,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -1133,14 +1129,11 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>154</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>67</v>
       </c>
@@ -1148,7 +1141,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -1156,7 +1149,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -1168,27 +1161,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1">
-      <c r="A6" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="27" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="28">
+        <v>155</v>
+      </c>
+      <c r="D6" s="27">
         <v>5</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -1196,14 +1189,11 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1211,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1219,14 +1209,11 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>154</v>
-      </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1234,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -1242,7 +1229,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="1">
         <v>8</v>
@@ -1263,7 +1250,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1284,7 +1271,7 @@
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -1305,7 +1292,7 @@
         <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
@@ -1326,7 +1313,7 @@
         <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -1347,7 +1334,7 @@
         <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="1">
         <v>5</v>
@@ -1368,7 +1355,7 @@
         <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -1389,7 +1376,7 @@
         <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="1">
         <v>7</v>
@@ -1402,7 +1389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -1410,7 +1397,7 @@
         <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="13">
         <v>1</v>
@@ -1420,7 +1407,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -1428,7 +1415,7 @@
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="13">
         <v>2</v>
@@ -1441,7 +1428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>127</v>
       </c>
@@ -1449,7 +1436,7 @@
         <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="13">
         <v>3</v>
@@ -1462,7 +1449,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -1470,7 +1457,7 @@
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="13">
         <v>4</v>
@@ -1483,7 +1470,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -1491,7 +1478,7 @@
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="13">
         <v>5</v>
@@ -1504,7 +1491,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -1512,7 +1499,7 @@
         <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D22" s="13">
         <v>6</v>
@@ -1533,7 +1520,7 @@
         <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D23" s="13">
         <v>1</v>
@@ -1551,7 +1538,7 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D24" s="13">
         <v>2</v>
@@ -1572,7 +1559,7 @@
         <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D25" s="13">
         <v>3</v>
@@ -1593,7 +1580,7 @@
         <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="13">
         <v>4</v>
@@ -1614,7 +1601,7 @@
         <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" s="13">
         <v>5</v>
@@ -1635,7 +1622,7 @@
         <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D28" s="13">
         <v>6</v>
@@ -1656,7 +1643,7 @@
         <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D29" s="13">
         <v>7</v>
@@ -1677,7 +1664,7 @@
         <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
@@ -1697,7 +1684,7 @@
         <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1717,13 +1704,13 @@
         <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
@@ -1740,7 +1727,7 @@
         <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D33" s="13">
         <v>1</v>
@@ -1749,7 +1736,7 @@
         <v>77</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1760,7 +1747,7 @@
         <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -1780,13 +1767,13 @@
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -1803,13 +1790,13 @@
         <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>9</v>
@@ -1818,7 +1805,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -1826,7 +1813,7 @@
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D37" s="13">
         <v>1</v>
@@ -1836,7 +1823,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -1844,7 +1831,7 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -1856,7 +1843,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -1864,7 +1851,7 @@
         <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
@@ -1877,7 +1864,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -1885,7 +1872,7 @@
         <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="1">
         <v>4</v>
@@ -1898,7 +1885,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>127</v>
       </c>
@@ -1906,7 +1893,7 @@
         <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -1918,7 +1905,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -1926,7 +1913,7 @@
         <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42">
         <v>6</v>
@@ -1938,7 +1925,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -1946,7 +1933,7 @@
         <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -1957,71 +1944,12 @@
       <c r="G43" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="18"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G43" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
     <filterColumn colId="0">
       <filters>
         <filter val="CUR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ESLP"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2038,8 +1966,8 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2064,7 +1992,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -2117,7 +2045,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -2126,7 +2054,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>17</v>
@@ -2165,7 +2093,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -2174,7 +2102,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
@@ -2213,7 +2141,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -2222,7 +2150,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
@@ -2263,7 +2191,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2272,7 +2200,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>17</v>
@@ -2311,7 +2239,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -2320,7 +2248,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>17</v>
@@ -2359,7 +2287,7 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -2368,7 +2296,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="4">
-        <v>45982</v>
+        <v>46001</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>17</v>
@@ -2407,7 +2335,7 @@
         <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -2460,7 +2388,7 @@
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -2508,7 +2436,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2556,7 +2484,7 @@
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -2604,7 +2532,7 @@
         <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -2654,7 +2582,7 @@
         <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -2702,7 +2630,7 @@
         <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>85</v>
@@ -2750,7 +2678,7 @@
         <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>85</v>
@@ -2798,7 +2726,7 @@
         <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>85</v>
@@ -2845,7 +2773,7 @@
         <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:16" hidden="1">
@@ -2856,7 +2784,7 @@
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>85</v>
@@ -2903,7 +2831,7 @@
         <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>85</v>
@@ -2950,7 +2878,7 @@
         <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>85</v>
@@ -2994,7 +2922,7 @@
         <v>127</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="12"/>
     </row>
@@ -3003,7 +2931,7 @@
         <v>127</v>
       </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" s="12"/>
     </row>
@@ -3015,7 +2943,7 @@
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>12</v>
@@ -3062,7 +2990,7 @@
         <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>136</v>
@@ -3076,10 +3004,10 @@
         <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>97</v>
@@ -3371,7 +3299,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C7"/>
+      <selection pane="bottomLeft" sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3393,7 +3321,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
@@ -3504,7 +3432,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>68</v>
@@ -3542,7 +3470,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>69</v>
@@ -3580,7 +3508,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>68</v>
@@ -3618,7 +3546,7 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>69</v>
@@ -3767,7 +3695,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -3806,7 +3734,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -3843,7 +3771,7 @@
         <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3880,7 +3808,7 @@
         <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>124</v>
@@ -3917,7 +3845,7 @@
         <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>102</v>
@@ -3955,7 +3883,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>100</v>
@@ -3991,7 +3919,7 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>101</v>
@@ -4027,7 +3955,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>108</v>
@@ -4063,7 +3991,7 @@
         <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>153</v>
@@ -4153,10 +4081,10 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>46001</v>
       </c>
       <c r="C2" t="s">
@@ -4185,10 +4113,10 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>46001</v>
       </c>
       <c r="C3" t="s">
@@ -4251,7 +4179,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>11</v>
@@ -4283,7 +4211,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -4315,7 +4243,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -4347,7 +4275,7 @@
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -4379,7 +4307,7 @@
         <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -4398,7 +4326,7 @@
         <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -4417,7 +4345,7 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -4451,7 +4379,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
         <v>103</v>
@@ -4490,7 +4418,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4514,7 +4442,7 @@
         <v>81</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>11</v>
@@ -4558,7 +4486,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -4602,7 +4530,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -4646,7 +4574,7 @@
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>130</v>
@@ -4690,7 +4618,7 @@
         <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>131</v>
@@ -4734,7 +4662,7 @@
         <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -4778,7 +4706,7 @@
         <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -4822,7 +4750,7 @@
         <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>94</v>
@@ -4866,7 +4794,7 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>99</v>
@@ -4910,7 +4838,7 @@
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>94</v>
@@ -4951,7 +4879,7 @@
         <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>99</v>
@@ -4995,7 +4923,7 @@
         <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>107</v>
@@ -5039,7 +4967,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>33</v>
@@ -5083,7 +5011,7 @@
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>107</v>
@@ -5124,7 +5052,7 @@
         <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Ahora las Transaction.notes tiene toda la info necesaria para persistir en la BD
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C73DCF9-604C-4561-A85F-0C45DC139401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F8A49-AF04-4BBF-B543-C44FA7DCC201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1470" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Transport" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Consume!$A$1:$O$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Consume!$A$1:$O$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$G$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$25</definedName>
@@ -1046,9 +1046,9 @@
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1966,8 +1966,8 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2037,7 +2037,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" hidden="1">
       <c r="A23" t="s">
         <v>127</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" hidden="1">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -3045,9 +3045,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q25" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CUR"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="ESLP"/>
+        <filter val="EAX"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3672,8 +3677,8 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4033,7 +4038,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4154,11 +4159,11 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:I8"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4202,6 +4207,9 @@
       <c r="J1" s="14" t="s">
         <v>49</v>
       </c>
+      <c r="K1" s="14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -4234,13 +4242,16 @@
       <c r="J2" s="2">
         <v>0.1</v>
       </c>
+      <c r="K2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>155</v>
@@ -4255,10 +4266,10 @@
         <v>138</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="H3" s="2">
-        <v>68862</v>
+        <v>15000</v>
       </c>
       <c r="I3" s="2">
         <v>5</v>
@@ -4266,13 +4277,16 @@
       <c r="J3" s="2">
         <v>0.1</v>
       </c>
+      <c r="K3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>155</v>
@@ -4280,24 +4294,14 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="2">
-        <v>15000</v>
-      </c>
-      <c r="I4" s="2">
-        <v>5</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="K4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
@@ -4315,6 +4319,9 @@
       <c r="F5" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="K5" t="s">
+        <v>108</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="2"/>
     </row>
@@ -4323,7 +4330,7 @@
         <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>155</v>
@@ -4331,8 +4338,26 @@
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>138</v>
+        <v>91</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>108</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="2"/>
@@ -4342,69 +4367,38 @@
         <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1000</v>
-      </c>
-      <c r="I7" s="2">
+        <v>148</v>
+      </c>
+      <c r="H7">
+        <v>832</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="J7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8">
-        <v>832</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8">
+      <c r="J7">
         <v>0.2</v>
       </c>
+      <c r="K7" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O8" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
+  <autoFilter ref="A1:O7" xr:uid="{3732F4A5-D4B8-494C-AA7D-B475C8F2D721}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4416,9 +4410,9 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14:E14"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5073,7 +5067,7 @@
         <v>80</v>
       </c>
       <c r="J15" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K15" s="2">
         <v>7.0000000000000007E-2</v>

</xml_diff>

<commit_message>
Log de errores funcionando: Ej. control de la cantidad a vender; Falta controlar las Excepciones
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F8A49-AF04-4BBF-B543-C44FA7DCC201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41BE921-2972-40DD-9788-A7A3D4879BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
-    <sheet name="Supply" sheetId="2" r:id="rId2"/>
-    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Sleeve" sheetId="7" r:id="rId4"/>
+    <sheet name="Sleeve" sheetId="7" r:id="rId2"/>
+    <sheet name="Supply" sheetId="2" r:id="rId3"/>
+    <sheet name="SupplyTrade" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="Trade" sheetId="4" r:id="rId5"/>
     <sheet name="Sell" sheetId="8" r:id="rId6"/>
     <sheet name="Consume" sheetId="6" r:id="rId7"/>
@@ -24,11 +24,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Consume!$A$1:$O$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$G$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sleeve!$A$1:$M$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Supply!$A$1:$Q$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Transport!$A$1:$N$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Flow!$A$1:$G$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sleeve!$A$1:$M$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Supply!$A$1:$Q$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Trade!$B$1:$L$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Transport!$A$1:$N$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="173">
   <si>
     <t>Order</t>
   </si>
@@ -534,6 +534,42 @@
   </si>
   <si>
     <t>JOIN_KEY</t>
+  </si>
+  <si>
+    <t>BEPC</t>
+  </si>
+  <si>
+    <t>BEPC-ECHI</t>
+  </si>
+  <si>
+    <t>Esentia-ECHI</t>
+  </si>
+  <si>
+    <t>T1-ECHI</t>
+  </si>
+  <si>
+    <t>T2-ECHI</t>
+  </si>
+  <si>
+    <t>ECHI-1</t>
+  </si>
+  <si>
+    <t>ECHI-2</t>
+  </si>
+  <si>
+    <t>T3-ECHI</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>KEYS</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>EPGN</t>
   </si>
 </sst>
 </file>
@@ -648,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -679,7 +715,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1044,11 +1079,11 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" activeCellId="2" sqref="G42 G39 G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1059,25 +1094,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1162,22 +1197,22 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>5</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1389,38 +1424,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <v>1</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1">
       <c r="A18" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <v>2</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
@@ -1428,20 +1463,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <v>3</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="1" t="s">
         <v>67</v>
       </c>
@@ -1449,20 +1484,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C20" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <v>4</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1470,20 +1505,20 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>155</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <v>5</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1491,20 +1526,20 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="12">
         <v>6</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1516,16 +1551,16 @@
       <c r="A23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C23" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <v>1</v>
       </c>
-      <c r="E23" s="13"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1534,16 +1569,16 @@
       <c r="A24" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C24" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <v>2</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1555,16 +1590,16 @@
       <c r="A25" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>155</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="12">
         <v>3</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1576,16 +1611,16 @@
       <c r="A26" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C26" t="s">
         <v>155</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <v>4</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1597,16 +1632,16 @@
       <c r="A27" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C27" t="s">
         <v>155</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="12">
         <v>5</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1618,16 +1653,16 @@
       <c r="A28" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C28" t="s">
         <v>155</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="12">
         <v>6</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1639,16 +1674,16 @@
       <c r="A29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C29" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="12">
         <v>7</v>
       </c>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1656,31 +1691,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="12">
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C31" t="s">
@@ -1696,11 +1731,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C32" t="s">
@@ -1719,31 +1754,31 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C34" t="s">
@@ -1759,11 +1794,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C35" t="s">
@@ -1782,11 +1817,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C36" t="s">
@@ -1805,151 +1840,186 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
-      </c>
-      <c r="D37" s="13">
+        <v>156</v>
+      </c>
+      <c r="D37" s="12">
         <v>1</v>
       </c>
-      <c r="E37" s="13"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="G37" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" t="s">
         <v>127</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>4</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" s="1">
+        <v>156</v>
+      </c>
+      <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" t="s">
+        <v>160</v>
+      </c>
       <c r="F40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>7</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1">
+      <c r="A42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42" s="13" t="s">
+      <c r="G42" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C42" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="13" t="s">
+      <c r="G43" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1">
+      <c r="A44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C43" t="s">
-        <v>155</v>
-      </c>
-      <c r="D43">
-        <v>7</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G44" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="G45" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G43" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:G44" xr:uid="{65D52CBE-03DA-4D86-9F67-E7962774C7A0}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="CUR"/>
+        <filter val="EAX"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1959,15 +2029,389 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
+  <sheetPr filterMode="1">
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="5" width="19.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="12" width="16.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" hidden="1">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" hidden="1">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="K3" s="10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="K5" s="10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" hidden="1">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" hidden="1">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:M9" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CUR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="3" tint="0.749992370372631"/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L7"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2021,13 +2465,13 @@
       <c r="L1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>119</v>
       </c>
       <c r="P1" s="11" t="s">
@@ -2054,7 +2498,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>17</v>
@@ -2074,13 +2518,13 @@
       <c r="L2" s="2">
         <v>18000</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N2" s="21">
+      <c r="N2" s="20">
         <v>0.03</v>
       </c>
-      <c r="O2" s="21"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="2" t="s">
         <v>30</v>
       </c>
@@ -2102,7 +2546,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
@@ -2122,13 +2566,13 @@
       <c r="L3" s="2">
         <v>15326</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="20">
         <v>0.03</v>
       </c>
-      <c r="O3" s="21"/>
+      <c r="O3" s="20"/>
       <c r="P3" s="2" t="s">
         <v>30</v>
       </c>
@@ -2150,7 +2594,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
@@ -2170,13 +2614,13 @@
       <c r="L4" s="2">
         <v>17000</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="20">
         <v>0.03</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>122</v>
       </c>
       <c r="P4" s="2" t="s">
@@ -2200,7 +2644,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>17</v>
@@ -2220,13 +2664,13 @@
       <c r="L5" s="2">
         <v>21645</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <v>2.37</v>
       </c>
-      <c r="N5" s="21">
+      <c r="N5" s="20">
         <v>0.03</v>
       </c>
-      <c r="O5" s="21"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2248,13 +2692,13 @@
         <v>14</v>
       </c>
       <c r="F6" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>21</v>
@@ -2268,13 +2712,13 @@
       <c r="L6">
         <v>43355</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="19">
         <v>0.77500000000000002</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="20">
         <v>0.03</v>
       </c>
-      <c r="O6" s="21"/>
+      <c r="O6" s="20"/>
       <c r="P6" s="2" t="s">
         <v>30</v>
       </c>
@@ -2296,7 +2740,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="4">
-        <v>46001</v>
+        <v>46010</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>17</v>
@@ -2316,18 +2760,18 @@
       <c r="L7">
         <v>25000</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="19">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="20">
         <v>0.03</v>
       </c>
-      <c r="O7" s="21"/>
+      <c r="O7" s="20"/>
       <c r="P7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -2340,47 +2784,47 @@
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>45982</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <v>-5000</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="19">
         <v>2.95</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="20">
         <v>0.03</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="15" t="s">
         <v>30</v>
       </c>
       <c r="Q8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -2414,21 +2858,21 @@
       <c r="K9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <v>10000</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="19">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="20">
         <v>0.03</v>
       </c>
-      <c r="O9" s="21"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -2462,21 +2906,21 @@
       <c r="K10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="15">
         <v>1000</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="20">
         <v>0.03</v>
       </c>
-      <c r="O10" s="21"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2510,21 +2954,21 @@
       <c r="K11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>2000</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="20">
         <v>0.03</v>
       </c>
-      <c r="O11" s="21"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -2558,23 +3002,23 @@
       <c r="K12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="15">
         <v>3000</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="18">
         <v>2.5750000000000002</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="20">
         <v>0.03</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="20" t="s">
         <v>122</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -2608,40 +3052,40 @@
       <c r="K13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="15">
         <v>4000</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="18">
         <v>2.37</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="20">
         <v>0.03</v>
       </c>
-      <c r="O13" s="21"/>
+      <c r="O13" s="20"/>
       <c r="P13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>127</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>155</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>86</v>
       </c>
       <c r="F14" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G14" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H14" t="s">
@@ -2668,28 +3112,28 @@
       <c r="P14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" hidden="1">
+      <c r="Q14" s="12"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>86</v>
       </c>
       <c r="F15" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G15" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H15" t="s">
@@ -2716,28 +3160,28 @@
       <c r="P15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Q15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" hidden="1">
+      <c r="Q15" s="12"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>86</v>
       </c>
       <c r="F16" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G16" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H16" t="s">
@@ -2761,47 +3205,86 @@
       <c r="N16">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="O16" s="20" t="s">
         <v>123</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>127</v>
       </c>
+      <c r="B17" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="C17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" hidden="1">
+      <c r="D17" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="4">
+        <v>46010</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17">
+        <v>25000</v>
+      </c>
+      <c r="M17">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="N17">
+        <v>0.04</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G18" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="14" t="s">
         <v>98</v>
       </c>
       <c r="J18" t="s">
@@ -2811,256 +3294,279 @@
         <v>25</v>
       </c>
       <c r="L18">
-        <v>25000</v>
+        <v>5300</v>
       </c>
       <c r="M18">
-        <v>2.5750000000000002</v>
+        <v>2.95</v>
       </c>
       <c r="N18">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F19" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G19" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="14" t="s">
         <v>98</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L19">
-        <v>5300</v>
+        <v>1000</v>
       </c>
       <c r="M19">
-        <v>2.95</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>83</v>
+      <c r="B20" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F20" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G20" s="15" t="s">
+        <v>46010</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="14" t="s">
         <v>98</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L20">
-        <v>1000</v>
+        <v>5300</v>
       </c>
       <c r="M20">
-        <v>2.5750000000000002</v>
+        <v>2.95</v>
       </c>
       <c r="N20">
-        <v>2.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" hidden="1">
-      <c r="A21" t="s">
-        <v>127</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>155</v>
       </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:16" hidden="1">
+      <c r="D21" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>127</v>
       </c>
+      <c r="B22" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="C22" t="s">
-        <v>155</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:16" hidden="1">
+        <v>157</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="4">
+        <v>46010</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J22" t="s">
+        <v>150</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <v>2000</v>
+      </c>
+      <c r="M22">
+        <v>1.9</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>103</v>
+      <c r="B23" t="s">
+        <v>109</v>
       </c>
       <c r="C23" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>97</v>
+      <c r="D23" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F23" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>87</v>
+        <v>46010</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>98</v>
+        <v>19</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="J23" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L23">
-        <v>5300</v>
-      </c>
-      <c r="M23">
-        <v>2.95</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
+      <c r="L23" s="2">
+        <v>45000</v>
+      </c>
+      <c r="M23" s="18">
+        <v>2.37</v>
+      </c>
+      <c r="N23" s="20">
+        <v>0.03</v>
+      </c>
+      <c r="O23" s="20"/>
       <c r="P23" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" hidden="1">
-      <c r="A24" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>82</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1">
-      <c r="A25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="4">
-        <v>45982</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="D24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="4">
+        <v>46010</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J25" t="s">
-        <v>150</v>
-      </c>
-      <c r="K25" s="2" t="s">
+      <c r="I24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L25">
-        <v>2000</v>
-      </c>
-      <c r="M25">
-        <v>1.9</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="L24">
+        <v>3700</v>
+      </c>
+      <c r="M24" s="19">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="N24" s="20">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="O24" s="20"/>
+      <c r="P24" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="G27" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q25" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CUR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="EAX"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q22" xr:uid="{FCB95230-BCA6-420A-B9F7-24F61506A35E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C52903-068A-4CF3-9AF2-E211C6D411FA}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -3295,390 +3801,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
-  <sheetPr filterMode="1">
-    <tabColor theme="8"/>
-  </sheetPr>
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="4" max="5" width="19.6328125" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="9" width="16.36328125" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="12" width="16.54296875" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1">
-      <c r="A2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1">
-      <c r="A3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="K3" s="10">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="K5" s="10">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" hidden="1">
-      <c r="A8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" hidden="1">
-      <c r="A9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:M9" xr:uid="{D0774D76-AF65-45E5-8F2B-082726EA3038}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CUR"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3714,16 +3846,16 @@
       <c r="G1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>117</v>
       </c>
       <c r="L1" s="11" t="s">
@@ -3753,13 +3885,13 @@
       <c r="G2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I2" s="23">
+      <c r="I2" s="22">
         <v>0.02</v>
       </c>
-      <c r="J2" s="23"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="8" t="s">
         <v>41</v>
       </c>
@@ -3790,13 +3922,13 @@
       <c r="G3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="22">
         <v>0.02</v>
       </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="8" t="s">
         <v>82</v>
       </c>
@@ -3809,7 +3941,7 @@
       <c r="A4" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C4" t="s">
@@ -3827,13 +3959,13 @@
       <c r="G4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <v>0.02</v>
       </c>
-      <c r="J4" s="23"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="10" t="s">
         <v>83</v>
       </c>
@@ -3846,7 +3978,7 @@
       <c r="A5" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C5" t="s">
@@ -3864,13 +3996,13 @@
       <c r="G5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="22">
         <v>0.02</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>121</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -3884,7 +4016,7 @@
       <c r="A6" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C6" t="s">
@@ -3902,13 +4034,13 @@
       <c r="G6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <v>0.02</v>
       </c>
-      <c r="J6" s="23"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="2" t="s">
         <v>83</v>
       </c>
@@ -3920,7 +4052,7 @@
       <c r="A7" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>83</v>
       </c>
       <c r="C7" t="s">
@@ -3938,13 +4070,13 @@
       <c r="G7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="22">
         <v>0.02</v>
       </c>
-      <c r="J7" s="23"/>
+      <c r="J7" s="22"/>
       <c r="K7" s="2" t="s">
         <v>83</v>
       </c>
@@ -3956,7 +4088,7 @@
       <c r="A8" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C8" t="s">
@@ -3974,13 +4106,13 @@
       <c r="G8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="22">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>0.02</v>
       </c>
-      <c r="J8" s="23"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="2" t="s">
         <v>103</v>
       </c>
@@ -3992,7 +4124,7 @@
       <c r="A9" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C9" t="s">
@@ -4010,13 +4142,13 @@
       <c r="G9" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="22">
         <v>0.03</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="J9" s="23"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="2" t="s">
         <v>103</v>
       </c>
@@ -4024,8 +4156,80 @@
         <v>34</v>
       </c>
     </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="22">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="I10" s="22">
+        <v>0.02</v>
+      </c>
+      <c r="J10" s="22"/>
+      <c r="K10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="22">
+        <v>0.03</v>
+      </c>
+      <c r="I11" s="22">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="K11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:L1" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}"/>
+  <autoFilter ref="B1:L11" xr:uid="{EFA7FC8B-D4AA-4F6A-9EF4-ABA3EB7A0379}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4037,8 +4241,8 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4086,11 +4290,11 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="24">
-        <v>46001</v>
+      <c r="B2" s="23">
+        <v>46010</v>
       </c>
       <c r="C2" t="s">
         <v>113</v>
@@ -4105,7 +4309,7 @@
         <v>141</v>
       </c>
       <c r="G2">
-        <v>60000</v>
+        <v>888888</v>
       </c>
       <c r="H2">
         <v>2.2999999999999998</v>
@@ -4118,11 +4322,11 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="24">
-        <v>46001</v>
+      <c r="B3" s="23">
+        <v>46010</v>
       </c>
       <c r="C3" t="s">
         <v>113</v>
@@ -4159,11 +4363,11 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4177,37 +4381,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4269,7 +4473,7 @@
         <v>82</v>
       </c>
       <c r="H3" s="2">
-        <v>15000</v>
+        <v>37032</v>
       </c>
       <c r="I3" s="2">
         <v>5</v>
@@ -4297,6 +4501,9 @@
       <c r="F4" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="H4">
+        <v>22000</v>
+      </c>
       <c r="K4" t="s">
         <v>108</v>
       </c>
@@ -4319,6 +4526,9 @@
       <c r="F5" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="H5">
+        <v>23000</v>
+      </c>
       <c r="K5" t="s">
         <v>108</v>
       </c>
@@ -4348,7 +4558,7 @@
         <v>83</v>
       </c>
       <c r="H6" s="2">
-        <v>1000</v>
+        <v>28000</v>
       </c>
       <c r="I6" s="2">
         <v>5</v>
@@ -4385,7 +4595,7 @@
         <v>148</v>
       </c>
       <c r="H7">
-        <v>832</v>
+        <v>78800</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -4395,6 +4605,41 @@
       </c>
       <c r="K7" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8">
+        <v>33429</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>0.2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4405,14 +4650,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4429,13 +4674,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>154</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -4472,7 +4717,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" hidden="1">
       <c r="A2" t="s">
         <v>127</v>
       </c>
@@ -4516,7 +4761,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" hidden="1">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -4560,7 +4805,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" hidden="1">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -4604,7 +4849,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" hidden="1">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -4648,7 +4893,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" hidden="1">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -4692,7 +4937,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" hidden="1">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -4736,7 +4981,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" hidden="1">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4780,7 +5025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" hidden="1">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -4824,7 +5069,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" hidden="1">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -4865,11 +5110,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" hidden="1">
       <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C11" t="s">
@@ -4909,11 +5154,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" hidden="1">
       <c r="A12" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C12" t="s">
@@ -4953,7 +5198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" hidden="1">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -4963,7 +5208,7 @@
       <c r="C13" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -4997,7 +5242,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" hidden="1">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -5038,7 +5283,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" hidden="1">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -5082,8 +5327,147 @@
         <v>149</v>
       </c>
     </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K17" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="K18" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N14" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}"/>
+  <autoFilter ref="A1:N18" xr:uid="{778E5712-A3A7-4E4F-A12E-D50E45D9EC40}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ECHI"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Limpieza de código -
</commit_message>
<xml_diff>
--- a/EscenarioSample.xlsx
+++ b/EscenarioSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cszit\source\repos\f#\Saavi\ComposeModel\ModeloSaavi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41BE921-2972-40DD-9788-A7A3D4879BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95271C4-C0BC-46AC-9B25-A55E89C67D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{4B6A4009-7EB0-4E3F-8301-FB82C7E984C4}"/>
   </bookViews>
@@ -4242,7 +4242,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4309,7 +4309,7 @@
         <v>141</v>
       </c>
       <c r="G2">
-        <v>888888</v>
+        <v>80000</v>
       </c>
       <c r="H2">
         <v>2.2999999999999998</v>

</xml_diff>